<commit_message>
edit xlsx files and added more notes
</commit_message>
<xml_diff>
--- a/xlsx/L1-1.xlsx
+++ b/xlsx/L1-1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\IQ-104\IHI-QI104\xls\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\QI-104\IHI-QI104\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55297D6F-5B32-432A-AF10-E252F8772355}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CDB141D-A529-43C7-9921-678B605631EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,15 +33,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
   <si>
     <t>Week</t>
   </si>
   <si>
     <t>perc</t>
-  </si>
-  <si>
-    <t>mean</t>
   </si>
   <si>
     <t>UCL</t>
@@ -53,7 +50,7 @@
     <t>std</t>
   </si>
   <si>
-    <t>ave</t>
+    <t>median</t>
   </si>
 </sst>
 </file>
@@ -193,7 +190,7 @@
           <c:yMode val="edge"/>
           <c:x val="8.6915196206534789E-2"/>
           <c:y val="0.11303614978826254"/>
-          <c:w val="0.81773126843992983"/>
+          <c:w val="0.81003526074392218"/>
           <c:h val="0.75163953446795906"/>
         </c:manualLayout>
       </c:layout>
@@ -774,160 +771,160 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="52"/>
                 <c:pt idx="0">
-                  <c:v>9.9251278074930056</c:v>
+                  <c:v>9.821688493254273</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.9251278074930056</c:v>
+                  <c:v>9.821688493254273</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9.9251278074930056</c:v>
+                  <c:v>9.821688493254273</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9.9251278074930056</c:v>
+                  <c:v>9.821688493254273</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9.9251278074930056</c:v>
+                  <c:v>9.821688493254273</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9.9251278074930056</c:v>
+                  <c:v>9.821688493254273</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9.9251278074930056</c:v>
+                  <c:v>9.821688493254273</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9.9251278074930056</c:v>
+                  <c:v>9.821688493254273</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9.9251278074930056</c:v>
+                  <c:v>9.821688493254273</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9.9251278074930056</c:v>
+                  <c:v>9.821688493254273</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>9.9251278074930056</c:v>
+                  <c:v>9.821688493254273</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>9.9251278074930056</c:v>
+                  <c:v>9.821688493254273</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>9.9251278074930056</c:v>
+                  <c:v>9.821688493254273</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>9.9251278074930056</c:v>
+                  <c:v>9.821688493254273</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>9.9251278074930056</c:v>
+                  <c:v>9.821688493254273</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>9.9251278074930056</c:v>
+                  <c:v>9.821688493254273</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>9.9251278074930056</c:v>
+                  <c:v>9.821688493254273</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>9.9251278074930056</c:v>
+                  <c:v>9.821688493254273</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>9.9251278074930056</c:v>
+                  <c:v>9.821688493254273</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>9.9251278074930056</c:v>
+                  <c:v>9.821688493254273</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>9.9251278074930056</c:v>
+                  <c:v>9.821688493254273</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>9.9251278074930056</c:v>
+                  <c:v>9.821688493254273</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>9.9251278074930056</c:v>
+                  <c:v>9.821688493254273</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>9.9251278074930056</c:v>
+                  <c:v>9.821688493254273</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>9.9251278074930056</c:v>
+                  <c:v>9.821688493254273</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>9.9251278074930056</c:v>
+                  <c:v>9.821688493254273</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>9.9251278074930056</c:v>
+                  <c:v>9.821688493254273</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>9.9251278074930056</c:v>
+                  <c:v>9.821688493254273</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>9.9251278074930056</c:v>
+                  <c:v>9.821688493254273</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>9.9251278074930056</c:v>
+                  <c:v>9.821688493254273</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>9.9251278074930056</c:v>
+                  <c:v>9.821688493254273</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>9.9251278074930056</c:v>
+                  <c:v>9.821688493254273</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>9.9251278074930056</c:v>
+                  <c:v>9.821688493254273</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>9.9251278074930056</c:v>
+                  <c:v>9.821688493254273</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>9.9251278074930056</c:v>
+                  <c:v>9.821688493254273</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>9.9251278074930056</c:v>
+                  <c:v>9.821688493254273</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>9.9251278074930056</c:v>
+                  <c:v>9.821688493254273</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>9.9251278074930056</c:v>
+                  <c:v>9.821688493254273</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>9.9251278074930056</c:v>
+                  <c:v>9.821688493254273</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>9.9251278074930056</c:v>
+                  <c:v>9.821688493254273</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>9.9251278074930056</c:v>
+                  <c:v>9.821688493254273</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>9.9251278074930056</c:v>
+                  <c:v>9.821688493254273</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>9.9251278074930056</c:v>
+                  <c:v>9.821688493254273</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>9.9251278074930056</c:v>
+                  <c:v>9.821688493254273</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>9.9251278074930056</c:v>
+                  <c:v>9.821688493254273</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>9.9251278074930056</c:v>
+                  <c:v>9.821688493254273</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>9.9251278074930056</c:v>
+                  <c:v>9.821688493254273</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>9.9251278074930056</c:v>
+                  <c:v>9.821688493254273</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>9.9251278074930056</c:v>
+                  <c:v>9.821688493254273</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>9.9251278074930056</c:v>
+                  <c:v>9.821688493254273</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>9.9251278074930056</c:v>
+                  <c:v>9.821688493254273</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>9.9251278074930056</c:v>
+                  <c:v>9.821688493254273</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1138,160 +1135,160 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="52"/>
                 <c:pt idx="0">
-                  <c:v>0.94252927549172583</c:v>
+                  <c:v>0.83908996125299318</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.94252927549172583</c:v>
+                  <c:v>0.83908996125299318</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.94252927549172583</c:v>
+                  <c:v>0.83908996125299318</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.94252927549172583</c:v>
+                  <c:v>0.83908996125299318</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.94252927549172583</c:v>
+                  <c:v>0.83908996125299318</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.94252927549172583</c:v>
+                  <c:v>0.83908996125299318</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.94252927549172583</c:v>
+                  <c:v>0.83908996125299318</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.94252927549172583</c:v>
+                  <c:v>0.83908996125299318</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.94252927549172583</c:v>
+                  <c:v>0.83908996125299318</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.94252927549172583</c:v>
+                  <c:v>0.83908996125299318</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.94252927549172583</c:v>
+                  <c:v>0.83908996125299318</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.94252927549172583</c:v>
+                  <c:v>0.83908996125299318</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.94252927549172583</c:v>
+                  <c:v>0.83908996125299318</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.94252927549172583</c:v>
+                  <c:v>0.83908996125299318</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.94252927549172583</c:v>
+                  <c:v>0.83908996125299318</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.94252927549172583</c:v>
+                  <c:v>0.83908996125299318</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.94252927549172583</c:v>
+                  <c:v>0.83908996125299318</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.94252927549172583</c:v>
+                  <c:v>0.83908996125299318</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.94252927549172583</c:v>
+                  <c:v>0.83908996125299318</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.94252927549172583</c:v>
+                  <c:v>0.83908996125299318</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.94252927549172583</c:v>
+                  <c:v>0.83908996125299318</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.94252927549172583</c:v>
+                  <c:v>0.83908996125299318</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.94252927549172583</c:v>
+                  <c:v>0.83908996125299318</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.94252927549172583</c:v>
+                  <c:v>0.83908996125299318</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.94252927549172583</c:v>
+                  <c:v>0.83908996125299318</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.94252927549172583</c:v>
+                  <c:v>0.83908996125299318</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.94252927549172583</c:v>
+                  <c:v>0.83908996125299318</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.94252927549172583</c:v>
+                  <c:v>0.83908996125299318</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.94252927549172583</c:v>
+                  <c:v>0.83908996125299318</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.94252927549172583</c:v>
+                  <c:v>0.83908996125299318</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.94252927549172583</c:v>
+                  <c:v>0.83908996125299318</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.94252927549172583</c:v>
+                  <c:v>0.83908996125299318</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.94252927549172583</c:v>
+                  <c:v>0.83908996125299318</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.94252927549172583</c:v>
+                  <c:v>0.83908996125299318</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.94252927549172583</c:v>
+                  <c:v>0.83908996125299318</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.94252927549172583</c:v>
+                  <c:v>0.83908996125299318</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.94252927549172583</c:v>
+                  <c:v>0.83908996125299318</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.94252927549172583</c:v>
+                  <c:v>0.83908996125299318</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.94252927549172583</c:v>
+                  <c:v>0.83908996125299318</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.94252927549172583</c:v>
+                  <c:v>0.83908996125299318</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.94252927549172583</c:v>
+                  <c:v>0.83908996125299318</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.94252927549172583</c:v>
+                  <c:v>0.83908996125299318</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0.94252927549172583</c:v>
+                  <c:v>0.83908996125299318</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0.94252927549172583</c:v>
+                  <c:v>0.83908996125299318</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.94252927549172583</c:v>
+                  <c:v>0.83908996125299318</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0.94252927549172583</c:v>
+                  <c:v>0.83908996125299318</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.94252927549172583</c:v>
+                  <c:v>0.83908996125299318</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0.94252927549172583</c:v>
+                  <c:v>0.83908996125299318</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0.94252927549172583</c:v>
+                  <c:v>0.83908996125299318</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.94252927549172583</c:v>
+                  <c:v>0.83908996125299318</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>0.94252927549172583</c:v>
+                  <c:v>0.83908996125299318</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>0.94252927549172583</c:v>
+                  <c:v>0.83908996125299318</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1312,7 +1309,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>mean</c:v>
+                  <c:v>median</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1502,160 +1499,160 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="52"/>
                 <c:pt idx="0">
-                  <c:v>5.4338285414923657</c:v>
+                  <c:v>5.3303892272536331</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.4338285414923657</c:v>
+                  <c:v>5.3303892272536331</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.4338285414923657</c:v>
+                  <c:v>5.3303892272536331</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.4338285414923657</c:v>
+                  <c:v>5.3303892272536331</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.4338285414923657</c:v>
+                  <c:v>5.3303892272536331</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.4338285414923657</c:v>
+                  <c:v>5.3303892272536331</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.4338285414923657</c:v>
+                  <c:v>5.3303892272536331</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5.4338285414923657</c:v>
+                  <c:v>5.3303892272536331</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5.4338285414923657</c:v>
+                  <c:v>5.3303892272536331</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5.4338285414923657</c:v>
+                  <c:v>5.3303892272536331</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5.4338285414923657</c:v>
+                  <c:v>5.3303892272536331</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>5.4338285414923657</c:v>
+                  <c:v>5.3303892272536331</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>5.4338285414923657</c:v>
+                  <c:v>5.3303892272536331</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>5.4338285414923657</c:v>
+                  <c:v>5.3303892272536331</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>5.4338285414923657</c:v>
+                  <c:v>5.3303892272536331</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>5.4338285414923657</c:v>
+                  <c:v>5.3303892272536331</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>5.4338285414923657</c:v>
+                  <c:v>5.3303892272536331</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>5.4338285414923657</c:v>
+                  <c:v>5.3303892272536331</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>5.4338285414923657</c:v>
+                  <c:v>5.3303892272536331</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>5.4338285414923657</c:v>
+                  <c:v>5.3303892272536331</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>5.4338285414923657</c:v>
+                  <c:v>5.3303892272536331</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>5.4338285414923657</c:v>
+                  <c:v>5.3303892272536331</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>5.4338285414923657</c:v>
+                  <c:v>5.3303892272536331</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>5.4338285414923657</c:v>
+                  <c:v>5.3303892272536331</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>5.4338285414923657</c:v>
+                  <c:v>5.3303892272536331</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>5.4338285414923657</c:v>
+                  <c:v>5.3303892272536331</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>5.4338285414923657</c:v>
+                  <c:v>5.3303892272536331</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>5.4338285414923657</c:v>
+                  <c:v>5.3303892272536331</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>5.4338285414923657</c:v>
+                  <c:v>5.3303892272536331</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>5.4338285414923657</c:v>
+                  <c:v>5.3303892272536331</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>5.4338285414923657</c:v>
+                  <c:v>5.3303892272536331</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>5.4338285414923657</c:v>
+                  <c:v>5.3303892272536331</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>5.4338285414923657</c:v>
+                  <c:v>5.3303892272536331</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>5.4338285414923657</c:v>
+                  <c:v>5.3303892272536331</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>5.4338285414923657</c:v>
+                  <c:v>5.3303892272536331</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>5.4338285414923657</c:v>
+                  <c:v>5.3303892272536331</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>5.4338285414923657</c:v>
+                  <c:v>5.3303892272536331</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>5.4338285414923657</c:v>
+                  <c:v>5.3303892272536331</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>5.4338285414923657</c:v>
+                  <c:v>5.3303892272536331</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>5.4338285414923657</c:v>
+                  <c:v>5.3303892272536331</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>5.4338285414923657</c:v>
+                  <c:v>5.3303892272536331</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>5.4338285414923657</c:v>
+                  <c:v>5.3303892272536331</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>5.4338285414923657</c:v>
+                  <c:v>5.3303892272536331</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>5.4338285414923657</c:v>
+                  <c:v>5.3303892272536331</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>5.4338285414923657</c:v>
+                  <c:v>5.3303892272536331</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>5.4338285414923657</c:v>
+                  <c:v>5.3303892272536331</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>5.4338285414923657</c:v>
+                  <c:v>5.3303892272536331</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>5.4338285414923657</c:v>
+                  <c:v>5.3303892272536331</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>5.4338285414923657</c:v>
+                  <c:v>5.3303892272536331</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>5.4338285414923657</c:v>
+                  <c:v>5.3303892272536331</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>5.4338285414923657</c:v>
+                  <c:v>5.3303892272536331</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>5.4338285414923657</c:v>
+                  <c:v>5.3303892272536331</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1668,7 +1665,6 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -2679,13 +2675,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>495299</xdr:colOff>
+      <xdr:colOff>447675</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>466724</xdr:colOff>
+      <xdr:colOff>476250</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
@@ -2702,8 +2698,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11534774" y="2428875"/>
-          <a:ext cx="581025" cy="238125"/>
+          <a:off x="11487150" y="2428875"/>
+          <a:ext cx="638175" cy="238125"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2731,7 +2727,7 @@
           <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr lang="en-US" sz="1100" b="1"/>
-            <a:t>Mean</a:t>
+            <a:t>Median</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -3007,7 +3003,7 @@
   <dimension ref="A1:H53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L29" sqref="L29"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3023,13 +3019,13 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -3040,19 +3036,19 @@
         <v>5.1530413089687421</v>
       </c>
       <c r="C2">
-        <f>AVERAGE(B:B)</f>
-        <v>5.4338285414923657</v>
+        <f>MEDIAN(B:B)</f>
+        <v>5.3303892272536331</v>
       </c>
       <c r="D2" s="2">
         <f>H$3+(H$2* 3 )</f>
-        <v>9.9251278074930056</v>
+        <v>9.821688493254273</v>
       </c>
       <c r="E2" s="2">
         <f>H$3-(H$2* 3 )</f>
-        <v>0.94252927549172583</v>
+        <v>0.83908996125299318</v>
       </c>
       <c r="G2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H2">
         <f>STDEV(B2:B53)</f>
@@ -3067,23 +3063,23 @@
         <v>4.0954059070930224</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C53" si="0">AVERAGE(B:B)</f>
-        <v>5.4338285414923657</v>
+        <f t="shared" ref="C3:C53" si="0">MEDIAN(B:B)</f>
+        <v>5.3303892272536331</v>
       </c>
       <c r="D3" s="2">
         <f t="shared" ref="D3:D53" si="1">H$3+(H$2* 3 )</f>
-        <v>9.9251278074930056</v>
+        <v>9.821688493254273</v>
       </c>
       <c r="E3" s="2">
         <f t="shared" ref="E3:E53" si="2">H$3-(H$2* 3 )</f>
-        <v>0.94252927549172583</v>
+        <v>0.83908996125299318</v>
       </c>
       <c r="G3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H3">
-        <f>AVERAGE(B:B)</f>
-        <v>5.4338285414923657</v>
+        <f>MEDIAN(B:B)</f>
+        <v>5.3303892272536331</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -3095,15 +3091,15 @@
       </c>
       <c r="C4">
         <f t="shared" si="0"/>
-        <v>5.4338285414923657</v>
+        <v>5.3303892272536331</v>
       </c>
       <c r="D4" s="2">
         <f t="shared" si="1"/>
-        <v>9.9251278074930056</v>
+        <v>9.821688493254273</v>
       </c>
       <c r="E4" s="2">
         <f t="shared" si="2"/>
-        <v>0.94252927549172583</v>
+        <v>0.83908996125299318</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -3115,15 +3111,15 @@
       </c>
       <c r="C5">
         <f t="shared" si="0"/>
-        <v>5.4338285414923657</v>
+        <v>5.3303892272536331</v>
       </c>
       <c r="D5" s="2">
         <f t="shared" si="1"/>
-        <v>9.9251278074930056</v>
+        <v>9.821688493254273</v>
       </c>
       <c r="E5" s="2">
         <f t="shared" si="2"/>
-        <v>0.94252927549172583</v>
+        <v>0.83908996125299318</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -3135,15 +3131,15 @@
       </c>
       <c r="C6">
         <f t="shared" si="0"/>
-        <v>5.4338285414923657</v>
+        <v>5.3303892272536331</v>
       </c>
       <c r="D6" s="2">
         <f t="shared" si="1"/>
-        <v>9.9251278074930056</v>
+        <v>9.821688493254273</v>
       </c>
       <c r="E6" s="2">
         <f t="shared" si="2"/>
-        <v>0.94252927549172583</v>
+        <v>0.83908996125299318</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -3155,15 +3151,15 @@
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>5.4338285414923657</v>
+        <v>5.3303892272536331</v>
       </c>
       <c r="D7" s="2">
         <f t="shared" si="1"/>
-        <v>9.9251278074930056</v>
+        <v>9.821688493254273</v>
       </c>
       <c r="E7" s="2">
         <f t="shared" si="2"/>
-        <v>0.94252927549172583</v>
+        <v>0.83908996125299318</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -3175,15 +3171,15 @@
       </c>
       <c r="C8">
         <f t="shared" si="0"/>
-        <v>5.4338285414923657</v>
+        <v>5.3303892272536331</v>
       </c>
       <c r="D8" s="2">
         <f t="shared" si="1"/>
-        <v>9.9251278074930056</v>
+        <v>9.821688493254273</v>
       </c>
       <c r="E8" s="2">
         <f t="shared" si="2"/>
-        <v>0.94252927549172583</v>
+        <v>0.83908996125299318</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -3195,15 +3191,15 @@
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
-        <v>5.4338285414923657</v>
+        <v>5.3303892272536331</v>
       </c>
       <c r="D9" s="2">
         <f t="shared" si="1"/>
-        <v>9.9251278074930056</v>
+        <v>9.821688493254273</v>
       </c>
       <c r="E9" s="2">
         <f t="shared" si="2"/>
-        <v>0.94252927549172583</v>
+        <v>0.83908996125299318</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -3215,15 +3211,15 @@
       </c>
       <c r="C10">
         <f t="shared" si="0"/>
-        <v>5.4338285414923657</v>
+        <v>5.3303892272536331</v>
       </c>
       <c r="D10" s="2">
         <f t="shared" si="1"/>
-        <v>9.9251278074930056</v>
+        <v>9.821688493254273</v>
       </c>
       <c r="E10" s="2">
         <f t="shared" si="2"/>
-        <v>0.94252927549172583</v>
+        <v>0.83908996125299318</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -3235,15 +3231,15 @@
       </c>
       <c r="C11">
         <f t="shared" si="0"/>
-        <v>5.4338285414923657</v>
+        <v>5.3303892272536331</v>
       </c>
       <c r="D11" s="2">
         <f t="shared" si="1"/>
-        <v>9.9251278074930056</v>
+        <v>9.821688493254273</v>
       </c>
       <c r="E11" s="2">
         <f t="shared" si="2"/>
-        <v>0.94252927549172583</v>
+        <v>0.83908996125299318</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -3255,15 +3251,15 @@
       </c>
       <c r="C12">
         <f t="shared" si="0"/>
-        <v>5.4338285414923657</v>
+        <v>5.3303892272536331</v>
       </c>
       <c r="D12" s="2">
         <f t="shared" si="1"/>
-        <v>9.9251278074930056</v>
+        <v>9.821688493254273</v>
       </c>
       <c r="E12" s="2">
         <f t="shared" si="2"/>
-        <v>0.94252927549172583</v>
+        <v>0.83908996125299318</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -3275,15 +3271,15 @@
       </c>
       <c r="C13">
         <f t="shared" si="0"/>
-        <v>5.4338285414923657</v>
+        <v>5.3303892272536331</v>
       </c>
       <c r="D13" s="2">
         <f t="shared" si="1"/>
-        <v>9.9251278074930056</v>
+        <v>9.821688493254273</v>
       </c>
       <c r="E13" s="2">
         <f t="shared" si="2"/>
-        <v>0.94252927549172583</v>
+        <v>0.83908996125299318</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -3295,15 +3291,15 @@
       </c>
       <c r="C14">
         <f t="shared" si="0"/>
-        <v>5.4338285414923657</v>
+        <v>5.3303892272536331</v>
       </c>
       <c r="D14" s="2">
         <f t="shared" si="1"/>
-        <v>9.9251278074930056</v>
+        <v>9.821688493254273</v>
       </c>
       <c r="E14" s="2">
         <f t="shared" si="2"/>
-        <v>0.94252927549172583</v>
+        <v>0.83908996125299318</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -3315,15 +3311,15 @@
       </c>
       <c r="C15">
         <f t="shared" si="0"/>
-        <v>5.4338285414923657</v>
+        <v>5.3303892272536331</v>
       </c>
       <c r="D15" s="2">
         <f t="shared" si="1"/>
-        <v>9.9251278074930056</v>
+        <v>9.821688493254273</v>
       </c>
       <c r="E15" s="2">
         <f t="shared" si="2"/>
-        <v>0.94252927549172583</v>
+        <v>0.83908996125299318</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -3335,15 +3331,15 @@
       </c>
       <c r="C16">
         <f t="shared" si="0"/>
-        <v>5.4338285414923657</v>
+        <v>5.3303892272536331</v>
       </c>
       <c r="D16" s="2">
         <f t="shared" si="1"/>
-        <v>9.9251278074930056</v>
+        <v>9.821688493254273</v>
       </c>
       <c r="E16" s="2">
         <f t="shared" si="2"/>
-        <v>0.94252927549172583</v>
+        <v>0.83908996125299318</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -3355,15 +3351,15 @@
       </c>
       <c r="C17">
         <f t="shared" si="0"/>
-        <v>5.4338285414923657</v>
+        <v>5.3303892272536331</v>
       </c>
       <c r="D17" s="2">
         <f t="shared" si="1"/>
-        <v>9.9251278074930056</v>
+        <v>9.821688493254273</v>
       </c>
       <c r="E17" s="2">
         <f t="shared" si="2"/>
-        <v>0.94252927549172583</v>
+        <v>0.83908996125299318</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -3375,15 +3371,15 @@
       </c>
       <c r="C18">
         <f t="shared" si="0"/>
-        <v>5.4338285414923657</v>
+        <v>5.3303892272536331</v>
       </c>
       <c r="D18" s="2">
         <f t="shared" si="1"/>
-        <v>9.9251278074930056</v>
+        <v>9.821688493254273</v>
       </c>
       <c r="E18" s="2">
         <f t="shared" si="2"/>
-        <v>0.94252927549172583</v>
+        <v>0.83908996125299318</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -3395,15 +3391,15 @@
       </c>
       <c r="C19">
         <f t="shared" si="0"/>
-        <v>5.4338285414923657</v>
+        <v>5.3303892272536331</v>
       </c>
       <c r="D19" s="2">
         <f t="shared" si="1"/>
-        <v>9.9251278074930056</v>
+        <v>9.821688493254273</v>
       </c>
       <c r="E19" s="2">
         <f t="shared" si="2"/>
-        <v>0.94252927549172583</v>
+        <v>0.83908996125299318</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -3415,15 +3411,15 @@
       </c>
       <c r="C20">
         <f t="shared" si="0"/>
-        <v>5.4338285414923657</v>
+        <v>5.3303892272536331</v>
       </c>
       <c r="D20" s="2">
         <f t="shared" si="1"/>
-        <v>9.9251278074930056</v>
+        <v>9.821688493254273</v>
       </c>
       <c r="E20" s="2">
         <f t="shared" si="2"/>
-        <v>0.94252927549172583</v>
+        <v>0.83908996125299318</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -3435,15 +3431,15 @@
       </c>
       <c r="C21">
         <f t="shared" si="0"/>
-        <v>5.4338285414923657</v>
+        <v>5.3303892272536331</v>
       </c>
       <c r="D21" s="2">
         <f t="shared" si="1"/>
-        <v>9.9251278074930056</v>
+        <v>9.821688493254273</v>
       </c>
       <c r="E21" s="2">
         <f t="shared" si="2"/>
-        <v>0.94252927549172583</v>
+        <v>0.83908996125299318</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -3455,15 +3451,15 @@
       </c>
       <c r="C22">
         <f t="shared" si="0"/>
-        <v>5.4338285414923657</v>
+        <v>5.3303892272536331</v>
       </c>
       <c r="D22" s="2">
         <f t="shared" si="1"/>
-        <v>9.9251278074930056</v>
+        <v>9.821688493254273</v>
       </c>
       <c r="E22" s="2">
         <f t="shared" si="2"/>
-        <v>0.94252927549172583</v>
+        <v>0.83908996125299318</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -3475,15 +3471,15 @@
       </c>
       <c r="C23">
         <f t="shared" si="0"/>
-        <v>5.4338285414923657</v>
+        <v>5.3303892272536331</v>
       </c>
       <c r="D23" s="2">
         <f t="shared" si="1"/>
-        <v>9.9251278074930056</v>
+        <v>9.821688493254273</v>
       </c>
       <c r="E23" s="2">
         <f t="shared" si="2"/>
-        <v>0.94252927549172583</v>
+        <v>0.83908996125299318</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -3495,15 +3491,15 @@
       </c>
       <c r="C24">
         <f t="shared" si="0"/>
-        <v>5.4338285414923657</v>
+        <v>5.3303892272536331</v>
       </c>
       <c r="D24" s="2">
         <f t="shared" si="1"/>
-        <v>9.9251278074930056</v>
+        <v>9.821688493254273</v>
       </c>
       <c r="E24" s="2">
         <f t="shared" si="2"/>
-        <v>0.94252927549172583</v>
+        <v>0.83908996125299318</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -3515,15 +3511,15 @@
       </c>
       <c r="C25">
         <f t="shared" si="0"/>
-        <v>5.4338285414923657</v>
+        <v>5.3303892272536331</v>
       </c>
       <c r="D25" s="2">
         <f t="shared" si="1"/>
-        <v>9.9251278074930056</v>
+        <v>9.821688493254273</v>
       </c>
       <c r="E25" s="2">
         <f t="shared" si="2"/>
-        <v>0.94252927549172583</v>
+        <v>0.83908996125299318</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -3535,15 +3531,15 @@
       </c>
       <c r="C26">
         <f t="shared" si="0"/>
-        <v>5.4338285414923657</v>
+        <v>5.3303892272536331</v>
       </c>
       <c r="D26" s="2">
         <f t="shared" si="1"/>
-        <v>9.9251278074930056</v>
+        <v>9.821688493254273</v>
       </c>
       <c r="E26" s="2">
         <f t="shared" si="2"/>
-        <v>0.94252927549172583</v>
+        <v>0.83908996125299318</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -3555,15 +3551,15 @@
       </c>
       <c r="C27">
         <f t="shared" si="0"/>
-        <v>5.4338285414923657</v>
+        <v>5.3303892272536331</v>
       </c>
       <c r="D27" s="2">
         <f t="shared" si="1"/>
-        <v>9.9251278074930056</v>
+        <v>9.821688493254273</v>
       </c>
       <c r="E27" s="2">
         <f t="shared" si="2"/>
-        <v>0.94252927549172583</v>
+        <v>0.83908996125299318</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -3575,15 +3571,15 @@
       </c>
       <c r="C28">
         <f t="shared" si="0"/>
-        <v>5.4338285414923657</v>
+        <v>5.3303892272536331</v>
       </c>
       <c r="D28" s="2">
         <f t="shared" si="1"/>
-        <v>9.9251278074930056</v>
+        <v>9.821688493254273</v>
       </c>
       <c r="E28" s="2">
         <f t="shared" si="2"/>
-        <v>0.94252927549172583</v>
+        <v>0.83908996125299318</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -3595,15 +3591,15 @@
       </c>
       <c r="C29">
         <f t="shared" si="0"/>
-        <v>5.4338285414923657</v>
+        <v>5.3303892272536331</v>
       </c>
       <c r="D29" s="2">
         <f t="shared" si="1"/>
-        <v>9.9251278074930056</v>
+        <v>9.821688493254273</v>
       </c>
       <c r="E29" s="2">
         <f t="shared" si="2"/>
-        <v>0.94252927549172583</v>
+        <v>0.83908996125299318</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -3615,15 +3611,15 @@
       </c>
       <c r="C30">
         <f t="shared" si="0"/>
-        <v>5.4338285414923657</v>
+        <v>5.3303892272536331</v>
       </c>
       <c r="D30" s="2">
         <f t="shared" si="1"/>
-        <v>9.9251278074930056</v>
+        <v>9.821688493254273</v>
       </c>
       <c r="E30" s="2">
         <f t="shared" si="2"/>
-        <v>0.94252927549172583</v>
+        <v>0.83908996125299318</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -3635,15 +3631,15 @@
       </c>
       <c r="C31">
         <f t="shared" si="0"/>
-        <v>5.4338285414923657</v>
+        <v>5.3303892272536331</v>
       </c>
       <c r="D31" s="2">
         <f t="shared" si="1"/>
-        <v>9.9251278074930056</v>
+        <v>9.821688493254273</v>
       </c>
       <c r="E31" s="2">
         <f t="shared" si="2"/>
-        <v>0.94252927549172583</v>
+        <v>0.83908996125299318</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -3655,15 +3651,15 @@
       </c>
       <c r="C32">
         <f t="shared" si="0"/>
-        <v>5.4338285414923657</v>
+        <v>5.3303892272536331</v>
       </c>
       <c r="D32" s="2">
         <f t="shared" si="1"/>
-        <v>9.9251278074930056</v>
+        <v>9.821688493254273</v>
       </c>
       <c r="E32" s="2">
         <f t="shared" si="2"/>
-        <v>0.94252927549172583</v>
+        <v>0.83908996125299318</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -3675,15 +3671,15 @@
       </c>
       <c r="C33">
         <f t="shared" si="0"/>
-        <v>5.4338285414923657</v>
+        <v>5.3303892272536331</v>
       </c>
       <c r="D33" s="2">
         <f t="shared" si="1"/>
-        <v>9.9251278074930056</v>
+        <v>9.821688493254273</v>
       </c>
       <c r="E33" s="2">
         <f t="shared" si="2"/>
-        <v>0.94252927549172583</v>
+        <v>0.83908996125299318</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -3695,15 +3691,15 @@
       </c>
       <c r="C34">
         <f t="shared" si="0"/>
-        <v>5.4338285414923657</v>
+        <v>5.3303892272536331</v>
       </c>
       <c r="D34" s="2">
         <f t="shared" si="1"/>
-        <v>9.9251278074930056</v>
+        <v>9.821688493254273</v>
       </c>
       <c r="E34" s="2">
         <f t="shared" si="2"/>
-        <v>0.94252927549172583</v>
+        <v>0.83908996125299318</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -3715,15 +3711,15 @@
       </c>
       <c r="C35">
         <f t="shared" si="0"/>
-        <v>5.4338285414923657</v>
+        <v>5.3303892272536331</v>
       </c>
       <c r="D35" s="2">
         <f t="shared" si="1"/>
-        <v>9.9251278074930056</v>
+        <v>9.821688493254273</v>
       </c>
       <c r="E35" s="2">
         <f t="shared" si="2"/>
-        <v>0.94252927549172583</v>
+        <v>0.83908996125299318</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -3735,15 +3731,15 @@
       </c>
       <c r="C36">
         <f t="shared" si="0"/>
-        <v>5.4338285414923657</v>
+        <v>5.3303892272536331</v>
       </c>
       <c r="D36" s="2">
         <f t="shared" si="1"/>
-        <v>9.9251278074930056</v>
+        <v>9.821688493254273</v>
       </c>
       <c r="E36" s="2">
         <f t="shared" si="2"/>
-        <v>0.94252927549172583</v>
+        <v>0.83908996125299318</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -3755,15 +3751,15 @@
       </c>
       <c r="C37">
         <f t="shared" si="0"/>
-        <v>5.4338285414923657</v>
+        <v>5.3303892272536331</v>
       </c>
       <c r="D37" s="2">
         <f t="shared" si="1"/>
-        <v>9.9251278074930056</v>
+        <v>9.821688493254273</v>
       </c>
       <c r="E37" s="2">
         <f t="shared" si="2"/>
-        <v>0.94252927549172583</v>
+        <v>0.83908996125299318</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -3775,15 +3771,15 @@
       </c>
       <c r="C38">
         <f t="shared" si="0"/>
-        <v>5.4338285414923657</v>
+        <v>5.3303892272536331</v>
       </c>
       <c r="D38" s="2">
         <f t="shared" si="1"/>
-        <v>9.9251278074930056</v>
+        <v>9.821688493254273</v>
       </c>
       <c r="E38" s="2">
         <f t="shared" si="2"/>
-        <v>0.94252927549172583</v>
+        <v>0.83908996125299318</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -3795,15 +3791,15 @@
       </c>
       <c r="C39">
         <f t="shared" si="0"/>
-        <v>5.4338285414923657</v>
+        <v>5.3303892272536331</v>
       </c>
       <c r="D39" s="2">
         <f t="shared" si="1"/>
-        <v>9.9251278074930056</v>
+        <v>9.821688493254273</v>
       </c>
       <c r="E39" s="2">
         <f t="shared" si="2"/>
-        <v>0.94252927549172583</v>
+        <v>0.83908996125299318</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -3815,15 +3811,15 @@
       </c>
       <c r="C40">
         <f t="shared" si="0"/>
-        <v>5.4338285414923657</v>
+        <v>5.3303892272536331</v>
       </c>
       <c r="D40" s="2">
         <f t="shared" si="1"/>
-        <v>9.9251278074930056</v>
+        <v>9.821688493254273</v>
       </c>
       <c r="E40" s="2">
         <f t="shared" si="2"/>
-        <v>0.94252927549172583</v>
+        <v>0.83908996125299318</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -3835,15 +3831,15 @@
       </c>
       <c r="C41">
         <f t="shared" si="0"/>
-        <v>5.4338285414923657</v>
+        <v>5.3303892272536331</v>
       </c>
       <c r="D41" s="2">
         <f t="shared" si="1"/>
-        <v>9.9251278074930056</v>
+        <v>9.821688493254273</v>
       </c>
       <c r="E41" s="2">
         <f t="shared" si="2"/>
-        <v>0.94252927549172583</v>
+        <v>0.83908996125299318</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -3855,15 +3851,15 @@
       </c>
       <c r="C42">
         <f t="shared" si="0"/>
-        <v>5.4338285414923657</v>
+        <v>5.3303892272536331</v>
       </c>
       <c r="D42" s="2">
         <f t="shared" si="1"/>
-        <v>9.9251278074930056</v>
+        <v>9.821688493254273</v>
       </c>
       <c r="E42" s="2">
         <f t="shared" si="2"/>
-        <v>0.94252927549172583</v>
+        <v>0.83908996125299318</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -3875,15 +3871,15 @@
       </c>
       <c r="C43">
         <f t="shared" si="0"/>
-        <v>5.4338285414923657</v>
+        <v>5.3303892272536331</v>
       </c>
       <c r="D43" s="2">
         <f t="shared" si="1"/>
-        <v>9.9251278074930056</v>
+        <v>9.821688493254273</v>
       </c>
       <c r="E43" s="2">
         <f t="shared" si="2"/>
-        <v>0.94252927549172583</v>
+        <v>0.83908996125299318</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -3895,15 +3891,15 @@
       </c>
       <c r="C44">
         <f t="shared" si="0"/>
-        <v>5.4338285414923657</v>
+        <v>5.3303892272536331</v>
       </c>
       <c r="D44" s="2">
         <f t="shared" si="1"/>
-        <v>9.9251278074930056</v>
+        <v>9.821688493254273</v>
       </c>
       <c r="E44" s="2">
         <f t="shared" si="2"/>
-        <v>0.94252927549172583</v>
+        <v>0.83908996125299318</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -3915,15 +3911,15 @@
       </c>
       <c r="C45">
         <f t="shared" si="0"/>
-        <v>5.4338285414923657</v>
+        <v>5.3303892272536331</v>
       </c>
       <c r="D45" s="2">
         <f t="shared" si="1"/>
-        <v>9.9251278074930056</v>
+        <v>9.821688493254273</v>
       </c>
       <c r="E45" s="2">
         <f t="shared" si="2"/>
-        <v>0.94252927549172583</v>
+        <v>0.83908996125299318</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -3935,15 +3931,15 @@
       </c>
       <c r="C46">
         <f t="shared" si="0"/>
-        <v>5.4338285414923657</v>
+        <v>5.3303892272536331</v>
       </c>
       <c r="D46" s="2">
         <f t="shared" si="1"/>
-        <v>9.9251278074930056</v>
+        <v>9.821688493254273</v>
       </c>
       <c r="E46" s="2">
         <f t="shared" si="2"/>
-        <v>0.94252927549172583</v>
+        <v>0.83908996125299318</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -3955,15 +3951,15 @@
       </c>
       <c r="C47">
         <f t="shared" si="0"/>
-        <v>5.4338285414923657</v>
+        <v>5.3303892272536331</v>
       </c>
       <c r="D47" s="2">
         <f t="shared" si="1"/>
-        <v>9.9251278074930056</v>
+        <v>9.821688493254273</v>
       </c>
       <c r="E47" s="2">
         <f t="shared" si="2"/>
-        <v>0.94252927549172583</v>
+        <v>0.83908996125299318</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -3975,15 +3971,15 @@
       </c>
       <c r="C48">
         <f t="shared" si="0"/>
-        <v>5.4338285414923657</v>
+        <v>5.3303892272536331</v>
       </c>
       <c r="D48" s="2">
         <f t="shared" si="1"/>
-        <v>9.9251278074930056</v>
+        <v>9.821688493254273</v>
       </c>
       <c r="E48" s="2">
         <f t="shared" si="2"/>
-        <v>0.94252927549172583</v>
+        <v>0.83908996125299318</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -3995,15 +3991,15 @@
       </c>
       <c r="C49">
         <f t="shared" si="0"/>
-        <v>5.4338285414923657</v>
+        <v>5.3303892272536331</v>
       </c>
       <c r="D49" s="2">
         <f t="shared" si="1"/>
-        <v>9.9251278074930056</v>
+        <v>9.821688493254273</v>
       </c>
       <c r="E49" s="2">
         <f t="shared" si="2"/>
-        <v>0.94252927549172583</v>
+        <v>0.83908996125299318</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -4015,15 +4011,15 @@
       </c>
       <c r="C50">
         <f t="shared" si="0"/>
-        <v>5.4338285414923657</v>
+        <v>5.3303892272536331</v>
       </c>
       <c r="D50" s="2">
         <f t="shared" si="1"/>
-        <v>9.9251278074930056</v>
+        <v>9.821688493254273</v>
       </c>
       <c r="E50" s="2">
         <f t="shared" si="2"/>
-        <v>0.94252927549172583</v>
+        <v>0.83908996125299318</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -4035,15 +4031,15 @@
       </c>
       <c r="C51">
         <f t="shared" si="0"/>
-        <v>5.4338285414923657</v>
+        <v>5.3303892272536331</v>
       </c>
       <c r="D51" s="2">
         <f t="shared" si="1"/>
-        <v>9.9251278074930056</v>
+        <v>9.821688493254273</v>
       </c>
       <c r="E51" s="2">
         <f t="shared" si="2"/>
-        <v>0.94252927549172583</v>
+        <v>0.83908996125299318</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -4055,15 +4051,15 @@
       </c>
       <c r="C52">
         <f t="shared" si="0"/>
-        <v>5.4338285414923657</v>
+        <v>5.3303892272536331</v>
       </c>
       <c r="D52" s="2">
         <f t="shared" si="1"/>
-        <v>9.9251278074930056</v>
+        <v>9.821688493254273</v>
       </c>
       <c r="E52" s="2">
         <f t="shared" si="2"/>
-        <v>0.94252927549172583</v>
+        <v>0.83908996125299318</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -4075,15 +4071,15 @@
       </c>
       <c r="C53">
         <f t="shared" si="0"/>
-        <v>5.4338285414923657</v>
+        <v>5.3303892272536331</v>
       </c>
       <c r="D53" s="2">
         <f t="shared" si="1"/>
-        <v>9.9251278074930056</v>
+        <v>9.821688493254273</v>
       </c>
       <c r="E53" s="2">
         <f t="shared" si="2"/>
-        <v>0.94252927549172583</v>
+        <v>0.83908996125299318</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed xlsx files, added more to L2
</commit_message>
<xml_diff>
--- a/xlsx/L1-1.xlsx
+++ b/xlsx/L1-1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\QI-104\IHI-QI104\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CDB141D-A529-43C7-9921-678B605631EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F47CAC60-EFC2-428D-931B-802E46805E51}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -86,9 +86,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -404,7 +403,7 @@
             <c:numRef>
               <c:f>'L1'!$B$2:$B$53</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="52"/>
                 <c:pt idx="0">
                   <c:v>5.1530413089687421</c:v>
@@ -1496,7 +1495,7 @@
             <c:numRef>
               <c:f>'L1'!$C$2:$C$53</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="52"/>
                 <c:pt idx="0">
                   <c:v>5.3303892272536331</c:v>
@@ -1868,7 +1867,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3003,7 +3002,7 @@
   <dimension ref="A1:H53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="V5" sqref="V5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3035,15 +3034,15 @@
       <c r="B2" s="1">
         <v>5.1530413089687421</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="1">
         <f>MEDIAN(B:B)</f>
         <v>5.3303892272536331</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="1">
         <f>H$3+(H$2* 3 )</f>
         <v>9.821688493254273</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="1">
         <f>H$3-(H$2* 3 )</f>
         <v>0.83908996125299318</v>
       </c>
@@ -3062,15 +3061,15 @@
       <c r="B3" s="1">
         <v>4.0954059070930224</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="1">
         <f t="shared" ref="C3:C53" si="0">MEDIAN(B:B)</f>
         <v>5.3303892272536331</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="1">
         <f t="shared" ref="D3:D53" si="1">H$3+(H$2* 3 )</f>
         <v>9.821688493254273</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="1">
         <f t="shared" ref="E3:E53" si="2">H$3-(H$2* 3 )</f>
         <v>0.83908996125299318</v>
       </c>
@@ -3089,15 +3088,15 @@
       <c r="B4" s="1">
         <v>4.5943494198374673</v>
       </c>
-      <c r="C4">
-        <f t="shared" si="0"/>
-        <v>5.3303892272536331</v>
-      </c>
-      <c r="D4" s="2">
-        <f t="shared" si="1"/>
-        <v>9.821688493254273</v>
-      </c>
-      <c r="E4" s="2">
+      <c r="C4" s="1">
+        <f t="shared" si="0"/>
+        <v>5.3303892272536331</v>
+      </c>
+      <c r="D4" s="1">
+        <f t="shared" si="1"/>
+        <v>9.821688493254273</v>
+      </c>
+      <c r="E4" s="1">
         <f t="shared" si="2"/>
         <v>0.83908996125299318</v>
       </c>
@@ -3109,15 +3108,15 @@
       <c r="B5" s="1">
         <v>7.6393267019633271</v>
       </c>
-      <c r="C5">
-        <f t="shared" si="0"/>
-        <v>5.3303892272536331</v>
-      </c>
-      <c r="D5" s="2">
-        <f t="shared" si="1"/>
-        <v>9.821688493254273</v>
-      </c>
-      <c r="E5" s="2">
+      <c r="C5" s="1">
+        <f t="shared" si="0"/>
+        <v>5.3303892272536331</v>
+      </c>
+      <c r="D5" s="1">
+        <f t="shared" si="1"/>
+        <v>9.821688493254273</v>
+      </c>
+      <c r="E5" s="1">
         <f t="shared" si="2"/>
         <v>0.83908996125299318</v>
       </c>
@@ -3129,15 +3128,15 @@
       <c r="B6" s="1">
         <v>3.1005619085876628</v>
       </c>
-      <c r="C6">
-        <f t="shared" si="0"/>
-        <v>5.3303892272536331</v>
-      </c>
-      <c r="D6" s="2">
-        <f t="shared" si="1"/>
-        <v>9.821688493254273</v>
-      </c>
-      <c r="E6" s="2">
+      <c r="C6" s="1">
+        <f t="shared" si="0"/>
+        <v>5.3303892272536331</v>
+      </c>
+      <c r="D6" s="1">
+        <f t="shared" si="1"/>
+        <v>9.821688493254273</v>
+      </c>
+      <c r="E6" s="1">
         <f t="shared" si="2"/>
         <v>0.83908996125299318</v>
       </c>
@@ -3149,15 +3148,15 @@
       <c r="B7" s="1">
         <v>5.3197840698422949</v>
       </c>
-      <c r="C7">
-        <f t="shared" si="0"/>
-        <v>5.3303892272536331</v>
-      </c>
-      <c r="D7" s="2">
-        <f t="shared" si="1"/>
-        <v>9.821688493254273</v>
-      </c>
-      <c r="E7" s="2">
+      <c r="C7" s="1">
+        <f t="shared" si="0"/>
+        <v>5.3303892272536331</v>
+      </c>
+      <c r="D7" s="1">
+        <f t="shared" si="1"/>
+        <v>9.821688493254273</v>
+      </c>
+      <c r="E7" s="1">
         <f t="shared" si="2"/>
         <v>0.83908996125299318</v>
       </c>
@@ -3169,15 +3168,15 @@
       <c r="B8" s="1">
         <v>4.0665241452581107</v>
       </c>
-      <c r="C8">
-        <f t="shared" si="0"/>
-        <v>5.3303892272536331</v>
-      </c>
-      <c r="D8" s="2">
-        <f t="shared" si="1"/>
-        <v>9.821688493254273</v>
-      </c>
-      <c r="E8" s="2">
+      <c r="C8" s="1">
+        <f t="shared" si="0"/>
+        <v>5.3303892272536331</v>
+      </c>
+      <c r="D8" s="1">
+        <f t="shared" si="1"/>
+        <v>9.821688493254273</v>
+      </c>
+      <c r="E8" s="1">
         <f t="shared" si="2"/>
         <v>0.83908996125299318</v>
       </c>
@@ -3189,15 +3188,15 @@
       <c r="B9" s="1">
         <v>7.2050144137075227</v>
       </c>
-      <c r="C9">
-        <f t="shared" si="0"/>
-        <v>5.3303892272536331</v>
-      </c>
-      <c r="D9" s="2">
-        <f t="shared" si="1"/>
-        <v>9.821688493254273</v>
-      </c>
-      <c r="E9" s="2">
+      <c r="C9" s="1">
+        <f t="shared" si="0"/>
+        <v>5.3303892272536331</v>
+      </c>
+      <c r="D9" s="1">
+        <f t="shared" si="1"/>
+        <v>9.821688493254273</v>
+      </c>
+      <c r="E9" s="1">
         <f t="shared" si="2"/>
         <v>0.83908996125299318</v>
       </c>
@@ -3209,15 +3208,15 @@
       <c r="B10" s="1">
         <v>5.3409943846649703</v>
       </c>
-      <c r="C10">
-        <f t="shared" si="0"/>
-        <v>5.3303892272536331</v>
-      </c>
-      <c r="D10" s="2">
-        <f t="shared" si="1"/>
-        <v>9.821688493254273</v>
-      </c>
-      <c r="E10" s="2">
+      <c r="C10" s="1">
+        <f t="shared" si="0"/>
+        <v>5.3303892272536331</v>
+      </c>
+      <c r="D10" s="1">
+        <f t="shared" si="1"/>
+        <v>9.821688493254273</v>
+      </c>
+      <c r="E10" s="1">
         <f t="shared" si="2"/>
         <v>0.83908996125299318</v>
       </c>
@@ -3229,15 +3228,15 @@
       <c r="B11" s="1">
         <v>7.1482092027772826</v>
       </c>
-      <c r="C11">
-        <f t="shared" si="0"/>
-        <v>5.3303892272536331</v>
-      </c>
-      <c r="D11" s="2">
-        <f t="shared" si="1"/>
-        <v>9.821688493254273</v>
-      </c>
-      <c r="E11" s="2">
+      <c r="C11" s="1">
+        <f t="shared" si="0"/>
+        <v>5.3303892272536331</v>
+      </c>
+      <c r="D11" s="1">
+        <f t="shared" si="1"/>
+        <v>9.821688493254273</v>
+      </c>
+      <c r="E11" s="1">
         <f t="shared" si="2"/>
         <v>0.83908996125299318</v>
       </c>
@@ -3249,15 +3248,15 @@
       <c r="B12" s="1">
         <v>3.8779734357075952</v>
       </c>
-      <c r="C12">
-        <f t="shared" si="0"/>
-        <v>5.3303892272536331</v>
-      </c>
-      <c r="D12" s="2">
-        <f t="shared" si="1"/>
-        <v>9.821688493254273</v>
-      </c>
-      <c r="E12" s="2">
+      <c r="C12" s="1">
+        <f t="shared" si="0"/>
+        <v>5.3303892272536331</v>
+      </c>
+      <c r="D12" s="1">
+        <f t="shared" si="1"/>
+        <v>9.821688493254273</v>
+      </c>
+      <c r="E12" s="1">
         <f t="shared" si="2"/>
         <v>0.83908996125299318</v>
       </c>
@@ -3269,15 +3268,15 @@
       <c r="B13" s="1">
         <v>3.3150046848766981</v>
       </c>
-      <c r="C13">
-        <f t="shared" si="0"/>
-        <v>5.3303892272536331</v>
-      </c>
-      <c r="D13" s="2">
-        <f t="shared" si="1"/>
-        <v>9.821688493254273</v>
-      </c>
-      <c r="E13" s="2">
+      <c r="C13" s="1">
+        <f t="shared" si="0"/>
+        <v>5.3303892272536331</v>
+      </c>
+      <c r="D13" s="1">
+        <f t="shared" si="1"/>
+        <v>9.821688493254273</v>
+      </c>
+      <c r="E13" s="1">
         <f t="shared" si="2"/>
         <v>0.83908996125299318</v>
       </c>
@@ -3289,15 +3288,15 @@
       <c r="B14" s="1">
         <v>7.555710089756869</v>
       </c>
-      <c r="C14">
-        <f t="shared" si="0"/>
-        <v>5.3303892272536331</v>
-      </c>
-      <c r="D14" s="2">
-        <f t="shared" si="1"/>
-        <v>9.821688493254273</v>
-      </c>
-      <c r="E14" s="2">
+      <c r="C14" s="1">
+        <f t="shared" si="0"/>
+        <v>5.3303892272536331</v>
+      </c>
+      <c r="D14" s="1">
+        <f t="shared" si="1"/>
+        <v>9.821688493254273</v>
+      </c>
+      <c r="E14" s="1">
         <f t="shared" si="2"/>
         <v>0.83908996125299318</v>
       </c>
@@ -3309,15 +3308,15 @@
       <c r="B15" s="1">
         <v>5.6396165788025368</v>
       </c>
-      <c r="C15">
-        <f t="shared" si="0"/>
-        <v>5.3303892272536331</v>
-      </c>
-      <c r="D15" s="2">
-        <f t="shared" si="1"/>
-        <v>9.821688493254273</v>
-      </c>
-      <c r="E15" s="2">
+      <c r="C15" s="1">
+        <f t="shared" si="0"/>
+        <v>5.3303892272536331</v>
+      </c>
+      <c r="D15" s="1">
+        <f t="shared" si="1"/>
+        <v>9.821688493254273</v>
+      </c>
+      <c r="E15" s="1">
         <f t="shared" si="2"/>
         <v>0.83908996125299318</v>
       </c>
@@ -3329,15 +3328,15 @@
       <c r="B16" s="1">
         <v>7.763306022315497</v>
       </c>
-      <c r="C16">
-        <f t="shared" si="0"/>
-        <v>5.3303892272536331</v>
-      </c>
-      <c r="D16" s="2">
-        <f t="shared" si="1"/>
-        <v>9.821688493254273</v>
-      </c>
-      <c r="E16" s="2">
+      <c r="C16" s="1">
+        <f t="shared" si="0"/>
+        <v>5.3303892272536331</v>
+      </c>
+      <c r="D16" s="1">
+        <f t="shared" si="1"/>
+        <v>9.821688493254273</v>
+      </c>
+      <c r="E16" s="1">
         <f t="shared" si="2"/>
         <v>0.83908996125299318</v>
       </c>
@@ -3349,15 +3348,15 @@
       <c r="B17" s="1">
         <v>5.4221224313444747</v>
       </c>
-      <c r="C17">
-        <f t="shared" si="0"/>
-        <v>5.3303892272536331</v>
-      </c>
-      <c r="D17" s="2">
-        <f t="shared" si="1"/>
-        <v>9.821688493254273</v>
-      </c>
-      <c r="E17" s="2">
+      <c r="C17" s="1">
+        <f t="shared" si="0"/>
+        <v>5.3303892272536331</v>
+      </c>
+      <c r="D17" s="1">
+        <f t="shared" si="1"/>
+        <v>9.821688493254273</v>
+      </c>
+      <c r="E17" s="1">
         <f t="shared" si="2"/>
         <v>0.83908996125299318</v>
       </c>
@@ -3369,15 +3368,15 @@
       <c r="B18" s="1">
         <v>5.7552291383214058</v>
       </c>
-      <c r="C18">
-        <f t="shared" si="0"/>
-        <v>5.3303892272536331</v>
-      </c>
-      <c r="D18" s="2">
-        <f t="shared" si="1"/>
-        <v>9.821688493254273</v>
-      </c>
-      <c r="E18" s="2">
+      <c r="C18" s="1">
+        <f t="shared" si="0"/>
+        <v>5.3303892272536331</v>
+      </c>
+      <c r="D18" s="1">
+        <f t="shared" si="1"/>
+        <v>9.821688493254273</v>
+      </c>
+      <c r="E18" s="1">
         <f t="shared" si="2"/>
         <v>0.83908996125299318</v>
       </c>
@@ -3389,15 +3388,15 @@
       <c r="B19" s="1">
         <v>6.8204787267303102</v>
       </c>
-      <c r="C19">
-        <f t="shared" si="0"/>
-        <v>5.3303892272536331</v>
-      </c>
-      <c r="D19" s="2">
-        <f t="shared" si="1"/>
-        <v>9.821688493254273</v>
-      </c>
-      <c r="E19" s="2">
+      <c r="C19" s="1">
+        <f t="shared" si="0"/>
+        <v>5.3303892272536331</v>
+      </c>
+      <c r="D19" s="1">
+        <f t="shared" si="1"/>
+        <v>9.821688493254273</v>
+      </c>
+      <c r="E19" s="1">
         <f t="shared" si="2"/>
         <v>0.83908996125299318</v>
       </c>
@@ -3409,15 +3408,15 @@
       <c r="B20" s="1">
         <v>4.0759926522959651</v>
       </c>
-      <c r="C20">
-        <f t="shared" si="0"/>
-        <v>5.3303892272536331</v>
-      </c>
-      <c r="D20" s="2">
-        <f t="shared" si="1"/>
-        <v>9.821688493254273</v>
-      </c>
-      <c r="E20" s="2">
+      <c r="C20" s="1">
+        <f t="shared" si="0"/>
+        <v>5.3303892272536331</v>
+      </c>
+      <c r="D20" s="1">
+        <f t="shared" si="1"/>
+        <v>9.821688493254273</v>
+      </c>
+      <c r="E20" s="1">
         <f t="shared" si="2"/>
         <v>0.83908996125299318</v>
       </c>
@@ -3429,15 +3428,15 @@
       <c r="B21" s="1">
         <v>3.2559808611488119</v>
       </c>
-      <c r="C21">
-        <f t="shared" si="0"/>
-        <v>5.3303892272536331</v>
-      </c>
-      <c r="D21" s="2">
-        <f t="shared" si="1"/>
-        <v>9.821688493254273</v>
-      </c>
-      <c r="E21" s="2">
+      <c r="C21" s="1">
+        <f t="shared" si="0"/>
+        <v>5.3303892272536331</v>
+      </c>
+      <c r="D21" s="1">
+        <f t="shared" si="1"/>
+        <v>9.821688493254273</v>
+      </c>
+      <c r="E21" s="1">
         <f t="shared" si="2"/>
         <v>0.83908996125299318</v>
       </c>
@@ -3449,15 +3448,15 @@
       <c r="B22" s="1">
         <v>3.6746491065817146</v>
       </c>
-      <c r="C22">
-        <f t="shared" si="0"/>
-        <v>5.3303892272536331</v>
-      </c>
-      <c r="D22" s="2">
-        <f t="shared" si="1"/>
-        <v>9.821688493254273</v>
-      </c>
-      <c r="E22" s="2">
+      <c r="C22" s="1">
+        <f t="shared" si="0"/>
+        <v>5.3303892272536331</v>
+      </c>
+      <c r="D22" s="1">
+        <f t="shared" si="1"/>
+        <v>9.821688493254273</v>
+      </c>
+      <c r="E22" s="1">
         <f t="shared" si="2"/>
         <v>0.83908996125299318</v>
       </c>
@@ -3469,15 +3468,15 @@
       <c r="B23" s="1">
         <v>6.8390627504248052</v>
       </c>
-      <c r="C23">
-        <f t="shared" si="0"/>
-        <v>5.3303892272536331</v>
-      </c>
-      <c r="D23" s="2">
-        <f t="shared" si="1"/>
-        <v>9.821688493254273</v>
-      </c>
-      <c r="E23" s="2">
+      <c r="C23" s="1">
+        <f t="shared" si="0"/>
+        <v>5.3303892272536331</v>
+      </c>
+      <c r="D23" s="1">
+        <f t="shared" si="1"/>
+        <v>9.821688493254273</v>
+      </c>
+      <c r="E23" s="1">
         <f t="shared" si="2"/>
         <v>0.83908996125299318</v>
       </c>
@@ -3489,15 +3488,15 @@
       <c r="B24" s="1">
         <v>6.4681828082838617</v>
       </c>
-      <c r="C24">
-        <f t="shared" si="0"/>
-        <v>5.3303892272536331</v>
-      </c>
-      <c r="D24" s="2">
-        <f t="shared" si="1"/>
-        <v>9.821688493254273</v>
-      </c>
-      <c r="E24" s="2">
+      <c r="C24" s="1">
+        <f t="shared" si="0"/>
+        <v>5.3303892272536331</v>
+      </c>
+      <c r="D24" s="1">
+        <f t="shared" si="1"/>
+        <v>9.821688493254273</v>
+      </c>
+      <c r="E24" s="1">
         <f t="shared" si="2"/>
         <v>0.83908996125299318</v>
       </c>
@@ -3509,15 +3508,15 @@
       <c r="B25" s="1">
         <v>7.8624827158895698</v>
       </c>
-      <c r="C25">
-        <f t="shared" si="0"/>
-        <v>5.3303892272536331</v>
-      </c>
-      <c r="D25" s="2">
-        <f t="shared" si="1"/>
-        <v>9.821688493254273</v>
-      </c>
-      <c r="E25" s="2">
+      <c r="C25" s="1">
+        <f t="shared" si="0"/>
+        <v>5.3303892272536331</v>
+      </c>
+      <c r="D25" s="1">
+        <f t="shared" si="1"/>
+        <v>9.821688493254273</v>
+      </c>
+      <c r="E25" s="1">
         <f t="shared" si="2"/>
         <v>0.83908996125299318</v>
       </c>
@@ -3529,15 +3528,15 @@
       <c r="B26" s="1">
         <v>7.0583269308621883</v>
       </c>
-      <c r="C26">
-        <f t="shared" si="0"/>
-        <v>5.3303892272536331</v>
-      </c>
-      <c r="D26" s="2">
-        <f t="shared" si="1"/>
-        <v>9.821688493254273</v>
-      </c>
-      <c r="E26" s="2">
+      <c r="C26" s="1">
+        <f t="shared" si="0"/>
+        <v>5.3303892272536331</v>
+      </c>
+      <c r="D26" s="1">
+        <f t="shared" si="1"/>
+        <v>9.821688493254273</v>
+      </c>
+      <c r="E26" s="1">
         <f t="shared" si="2"/>
         <v>0.83908996125299318</v>
       </c>
@@ -3549,15 +3548,15 @@
       <c r="B27" s="1">
         <v>3.5430589252308038</v>
       </c>
-      <c r="C27">
-        <f t="shared" si="0"/>
-        <v>5.3303892272536331</v>
-      </c>
-      <c r="D27" s="2">
-        <f t="shared" si="1"/>
-        <v>9.821688493254273</v>
-      </c>
-      <c r="E27" s="2">
+      <c r="C27" s="1">
+        <f t="shared" si="0"/>
+        <v>5.3303892272536331</v>
+      </c>
+      <c r="D27" s="1">
+        <f t="shared" si="1"/>
+        <v>9.821688493254273</v>
+      </c>
+      <c r="E27" s="1">
         <f t="shared" si="2"/>
         <v>0.83908996125299318</v>
       </c>
@@ -3569,15 +3568,15 @@
       <c r="B28" s="1">
         <v>3.9447878457229946</v>
       </c>
-      <c r="C28">
-        <f t="shared" si="0"/>
-        <v>5.3303892272536331</v>
-      </c>
-      <c r="D28" s="2">
-        <f t="shared" si="1"/>
-        <v>9.821688493254273</v>
-      </c>
-      <c r="E28" s="2">
+      <c r="C28" s="1">
+        <f t="shared" si="0"/>
+        <v>5.3303892272536331</v>
+      </c>
+      <c r="D28" s="1">
+        <f t="shared" si="1"/>
+        <v>9.821688493254273</v>
+      </c>
+      <c r="E28" s="1">
         <f t="shared" si="2"/>
         <v>0.83908996125299318</v>
       </c>
@@ -3589,15 +3588,15 @@
       <c r="B29" s="1">
         <v>6.3924618657014882</v>
       </c>
-      <c r="C29">
-        <f t="shared" si="0"/>
-        <v>5.3303892272536331</v>
-      </c>
-      <c r="D29" s="2">
-        <f t="shared" si="1"/>
-        <v>9.821688493254273</v>
-      </c>
-      <c r="E29" s="2">
+      <c r="C29" s="1">
+        <f t="shared" si="0"/>
+        <v>5.3303892272536331</v>
+      </c>
+      <c r="D29" s="1">
+        <f t="shared" si="1"/>
+        <v>9.821688493254273</v>
+      </c>
+      <c r="E29" s="1">
         <f t="shared" si="2"/>
         <v>0.83908996125299318</v>
       </c>
@@ -3609,15 +3608,15 @@
       <c r="B30" s="1">
         <v>3.214380551268861</v>
       </c>
-      <c r="C30">
-        <f t="shared" si="0"/>
-        <v>5.3303892272536331</v>
-      </c>
-      <c r="D30" s="2">
-        <f t="shared" si="1"/>
-        <v>9.821688493254273</v>
-      </c>
-      <c r="E30" s="2">
+      <c r="C30" s="1">
+        <f t="shared" si="0"/>
+        <v>5.3303892272536331</v>
+      </c>
+      <c r="D30" s="1">
+        <f t="shared" si="1"/>
+        <v>9.821688493254273</v>
+      </c>
+      <c r="E30" s="1">
         <f t="shared" si="2"/>
         <v>0.83908996125299318</v>
       </c>
@@ -3629,15 +3628,15 @@
       <c r="B31" s="1">
         <v>5.8113515624273209</v>
       </c>
-      <c r="C31">
-        <f t="shared" si="0"/>
-        <v>5.3303892272536331</v>
-      </c>
-      <c r="D31" s="2">
-        <f t="shared" si="1"/>
-        <v>9.821688493254273</v>
-      </c>
-      <c r="E31" s="2">
+      <c r="C31" s="1">
+        <f t="shared" si="0"/>
+        <v>5.3303892272536331</v>
+      </c>
+      <c r="D31" s="1">
+        <f t="shared" si="1"/>
+        <v>9.821688493254273</v>
+      </c>
+      <c r="E31" s="1">
         <f t="shared" si="2"/>
         <v>0.83908996125299318</v>
       </c>
@@ -3649,15 +3648,15 @@
       <c r="B32" s="1">
         <v>6.6638751184812497</v>
       </c>
-      <c r="C32">
-        <f t="shared" si="0"/>
-        <v>5.3303892272536331</v>
-      </c>
-      <c r="D32" s="2">
-        <f t="shared" si="1"/>
-        <v>9.821688493254273</v>
-      </c>
-      <c r="E32" s="2">
+      <c r="C32" s="1">
+        <f t="shared" si="0"/>
+        <v>5.3303892272536331</v>
+      </c>
+      <c r="D32" s="1">
+        <f t="shared" si="1"/>
+        <v>9.821688493254273</v>
+      </c>
+      <c r="E32" s="1">
         <f t="shared" si="2"/>
         <v>0.83908996125299318</v>
       </c>
@@ -3669,15 +3668,15 @@
       <c r="B33" s="1">
         <v>7.6934256538946606</v>
       </c>
-      <c r="C33">
-        <f t="shared" si="0"/>
-        <v>5.3303892272536331</v>
-      </c>
-      <c r="D33" s="2">
-        <f t="shared" si="1"/>
-        <v>9.821688493254273</v>
-      </c>
-      <c r="E33" s="2">
+      <c r="C33" s="1">
+        <f t="shared" si="0"/>
+        <v>5.3303892272536331</v>
+      </c>
+      <c r="D33" s="1">
+        <f t="shared" si="1"/>
+        <v>9.821688493254273</v>
+      </c>
+      <c r="E33" s="1">
         <f t="shared" si="2"/>
         <v>0.83908996125299318</v>
       </c>
@@ -3689,15 +3688,15 @@
       <c r="B34" s="1">
         <v>3.916898026992877</v>
       </c>
-      <c r="C34">
-        <f t="shared" si="0"/>
-        <v>5.3303892272536331</v>
-      </c>
-      <c r="D34" s="2">
-        <f t="shared" si="1"/>
-        <v>9.821688493254273</v>
-      </c>
-      <c r="E34" s="2">
+      <c r="C34" s="1">
+        <f t="shared" si="0"/>
+        <v>5.3303892272536331</v>
+      </c>
+      <c r="D34" s="1">
+        <f t="shared" si="1"/>
+        <v>9.821688493254273</v>
+      </c>
+      <c r="E34" s="1">
         <f t="shared" si="2"/>
         <v>0.83908996125299318</v>
       </c>
@@ -3709,15 +3708,15 @@
       <c r="B35" s="1">
         <v>5.9338158623080286</v>
       </c>
-      <c r="C35">
-        <f t="shared" si="0"/>
-        <v>5.3303892272536331</v>
-      </c>
-      <c r="D35" s="2">
-        <f t="shared" si="1"/>
-        <v>9.821688493254273</v>
-      </c>
-      <c r="E35" s="2">
+      <c r="C35" s="1">
+        <f t="shared" si="0"/>
+        <v>5.3303892272536331</v>
+      </c>
+      <c r="D35" s="1">
+        <f t="shared" si="1"/>
+        <v>9.821688493254273</v>
+      </c>
+      <c r="E35" s="1">
         <f t="shared" si="2"/>
         <v>0.83908996125299318</v>
       </c>
@@ -3729,15 +3728,15 @@
       <c r="B36" s="1">
         <v>5.1056158240019922</v>
       </c>
-      <c r="C36">
-        <f t="shared" si="0"/>
-        <v>5.3303892272536331</v>
-      </c>
-      <c r="D36" s="2">
-        <f t="shared" si="1"/>
-        <v>9.821688493254273</v>
-      </c>
-      <c r="E36" s="2">
+      <c r="C36" s="1">
+        <f t="shared" si="0"/>
+        <v>5.3303892272536331</v>
+      </c>
+      <c r="D36" s="1">
+        <f t="shared" si="1"/>
+        <v>9.821688493254273</v>
+      </c>
+      <c r="E36" s="1">
         <f t="shared" si="2"/>
         <v>0.83908996125299318</v>
       </c>
@@ -3749,15 +3748,15 @@
       <c r="B37" s="1">
         <v>4.0812833558478143</v>
       </c>
-      <c r="C37">
-        <f t="shared" si="0"/>
-        <v>5.3303892272536331</v>
-      </c>
-      <c r="D37" s="2">
-        <f t="shared" si="1"/>
-        <v>9.821688493254273</v>
-      </c>
-      <c r="E37" s="2">
+      <c r="C37" s="1">
+        <f t="shared" si="0"/>
+        <v>5.3303892272536331</v>
+      </c>
+      <c r="D37" s="1">
+        <f t="shared" si="1"/>
+        <v>9.821688493254273</v>
+      </c>
+      <c r="E37" s="1">
         <f t="shared" si="2"/>
         <v>0.83908996125299318</v>
       </c>
@@ -3769,15 +3768,15 @@
       <c r="B38" s="1">
         <v>6.2744022206576773</v>
       </c>
-      <c r="C38">
-        <f t="shared" si="0"/>
-        <v>5.3303892272536331</v>
-      </c>
-      <c r="D38" s="2">
-        <f t="shared" si="1"/>
-        <v>9.821688493254273</v>
-      </c>
-      <c r="E38" s="2">
+      <c r="C38" s="1">
+        <f t="shared" si="0"/>
+        <v>5.3303892272536331</v>
+      </c>
+      <c r="D38" s="1">
+        <f t="shared" si="1"/>
+        <v>9.821688493254273</v>
+      </c>
+      <c r="E38" s="1">
         <f t="shared" si="2"/>
         <v>0.83908996125299318</v>
       </c>
@@ -3789,15 +3788,15 @@
       <c r="B39" s="1">
         <v>3.8078765542056314</v>
       </c>
-      <c r="C39">
-        <f t="shared" si="0"/>
-        <v>5.3303892272536331</v>
-      </c>
-      <c r="D39" s="2">
-        <f t="shared" si="1"/>
-        <v>9.821688493254273</v>
-      </c>
-      <c r="E39" s="2">
+      <c r="C39" s="1">
+        <f t="shared" si="0"/>
+        <v>5.3303892272536331</v>
+      </c>
+      <c r="D39" s="1">
+        <f t="shared" si="1"/>
+        <v>9.821688493254273</v>
+      </c>
+      <c r="E39" s="1">
         <f t="shared" si="2"/>
         <v>0.83908996125299318</v>
       </c>
@@ -3809,15 +3808,15 @@
       <c r="B40" s="1">
         <v>6.8501538724696456</v>
       </c>
-      <c r="C40">
-        <f t="shared" si="0"/>
-        <v>5.3303892272536331</v>
-      </c>
-      <c r="D40" s="2">
-        <f t="shared" si="1"/>
-        <v>9.821688493254273</v>
-      </c>
-      <c r="E40" s="2">
+      <c r="C40" s="1">
+        <f t="shared" si="0"/>
+        <v>5.3303892272536331</v>
+      </c>
+      <c r="D40" s="1">
+        <f t="shared" si="1"/>
+        <v>9.821688493254273</v>
+      </c>
+      <c r="E40" s="1">
         <f t="shared" si="2"/>
         <v>0.83908996125299318</v>
       </c>
@@ -3829,15 +3828,15 @@
       <c r="B41" s="1">
         <v>4.828880642366161</v>
       </c>
-      <c r="C41">
-        <f t="shared" si="0"/>
-        <v>5.3303892272536331</v>
-      </c>
-      <c r="D41" s="2">
-        <f t="shared" si="1"/>
-        <v>9.821688493254273</v>
-      </c>
-      <c r="E41" s="2">
+      <c r="C41" s="1">
+        <f t="shared" si="0"/>
+        <v>5.3303892272536331</v>
+      </c>
+      <c r="D41" s="1">
+        <f t="shared" si="1"/>
+        <v>9.821688493254273</v>
+      </c>
+      <c r="E41" s="1">
         <f t="shared" si="2"/>
         <v>0.83908996125299318</v>
       </c>
@@ -3849,15 +3848,15 @@
       <c r="B42" s="1">
         <v>6.9640933577555009</v>
       </c>
-      <c r="C42">
-        <f t="shared" si="0"/>
-        <v>5.3303892272536331</v>
-      </c>
-      <c r="D42" s="2">
-        <f t="shared" si="1"/>
-        <v>9.821688493254273</v>
-      </c>
-      <c r="E42" s="2">
+      <c r="C42" s="1">
+        <f t="shared" si="0"/>
+        <v>5.3303892272536331</v>
+      </c>
+      <c r="D42" s="1">
+        <f t="shared" si="1"/>
+        <v>9.821688493254273</v>
+      </c>
+      <c r="E42" s="1">
         <f t="shared" si="2"/>
         <v>0.83908996125299318</v>
       </c>
@@ -3869,15 +3868,15 @@
       <c r="B43" s="1">
         <v>6.6508871810430383</v>
       </c>
-      <c r="C43">
-        <f t="shared" si="0"/>
-        <v>5.3303892272536331</v>
-      </c>
-      <c r="D43" s="2">
-        <f t="shared" si="1"/>
-        <v>9.821688493254273</v>
-      </c>
-      <c r="E43" s="2">
+      <c r="C43" s="1">
+        <f t="shared" si="0"/>
+        <v>5.3303892272536331</v>
+      </c>
+      <c r="D43" s="1">
+        <f t="shared" si="1"/>
+        <v>9.821688493254273</v>
+      </c>
+      <c r="E43" s="1">
         <f t="shared" si="2"/>
         <v>0.83908996125299318</v>
       </c>
@@ -3889,15 +3888,15 @@
       <c r="B44" s="1">
         <v>4.2006919136498544</v>
       </c>
-      <c r="C44">
-        <f t="shared" si="0"/>
-        <v>5.3303892272536331</v>
-      </c>
-      <c r="D44" s="2">
-        <f t="shared" si="1"/>
-        <v>9.821688493254273</v>
-      </c>
-      <c r="E44" s="2">
+      <c r="C44" s="1">
+        <f t="shared" si="0"/>
+        <v>5.3303892272536331</v>
+      </c>
+      <c r="D44" s="1">
+        <f t="shared" si="1"/>
+        <v>9.821688493254273</v>
+      </c>
+      <c r="E44" s="1">
         <f t="shared" si="2"/>
         <v>0.83908996125299318</v>
       </c>
@@ -3909,15 +3908,15 @@
       <c r="B45" s="1">
         <v>3.0337798814707018</v>
       </c>
-      <c r="C45">
-        <f t="shared" si="0"/>
-        <v>5.3303892272536331</v>
-      </c>
-      <c r="D45" s="2">
-        <f t="shared" si="1"/>
-        <v>9.821688493254273</v>
-      </c>
-      <c r="E45" s="2">
+      <c r="C45" s="1">
+        <f t="shared" si="0"/>
+        <v>5.3303892272536331</v>
+      </c>
+      <c r="D45" s="1">
+        <f t="shared" si="1"/>
+        <v>9.821688493254273</v>
+      </c>
+      <c r="E45" s="1">
         <f t="shared" si="2"/>
         <v>0.83908996125299318</v>
       </c>
@@ -3929,15 +3928,15 @@
       <c r="B46" s="1">
         <v>6.9848003153180667</v>
       </c>
-      <c r="C46">
-        <f t="shared" si="0"/>
-        <v>5.3303892272536331</v>
-      </c>
-      <c r="D46" s="2">
-        <f t="shared" si="1"/>
-        <v>9.821688493254273</v>
-      </c>
-      <c r="E46" s="2">
+      <c r="C46" s="1">
+        <f t="shared" si="0"/>
+        <v>5.3303892272536331</v>
+      </c>
+      <c r="D46" s="1">
+        <f t="shared" si="1"/>
+        <v>9.821688493254273</v>
+      </c>
+      <c r="E46" s="1">
         <f t="shared" si="2"/>
         <v>0.83908996125299318</v>
       </c>
@@ -3949,15 +3948,15 @@
       <c r="B47" s="1">
         <v>3.5676222447039212</v>
       </c>
-      <c r="C47">
-        <f t="shared" si="0"/>
-        <v>5.3303892272536331</v>
-      </c>
-      <c r="D47" s="2">
-        <f t="shared" si="1"/>
-        <v>9.821688493254273</v>
-      </c>
-      <c r="E47" s="2">
+      <c r="C47" s="1">
+        <f t="shared" si="0"/>
+        <v>5.3303892272536331</v>
+      </c>
+      <c r="D47" s="1">
+        <f t="shared" si="1"/>
+        <v>9.821688493254273</v>
+      </c>
+      <c r="E47" s="1">
         <f t="shared" si="2"/>
         <v>0.83908996125299318</v>
       </c>
@@ -3969,15 +3968,15 @@
       <c r="B48" s="1">
         <v>5.2882081484461736</v>
       </c>
-      <c r="C48">
-        <f t="shared" si="0"/>
-        <v>5.3303892272536331</v>
-      </c>
-      <c r="D48" s="2">
-        <f t="shared" si="1"/>
-        <v>9.821688493254273</v>
-      </c>
-      <c r="E48" s="2">
+      <c r="C48" s="1">
+        <f t="shared" si="0"/>
+        <v>5.3303892272536331</v>
+      </c>
+      <c r="D48" s="1">
+        <f t="shared" si="1"/>
+        <v>9.821688493254273</v>
+      </c>
+      <c r="E48" s="1">
         <f t="shared" si="2"/>
         <v>0.83908996125299318</v>
       </c>
@@ -3989,15 +3988,15 @@
       <c r="B49" s="1">
         <v>7.2069367492096408</v>
       </c>
-      <c r="C49">
-        <f t="shared" si="0"/>
-        <v>5.3303892272536331</v>
-      </c>
-      <c r="D49" s="2">
-        <f t="shared" si="1"/>
-        <v>9.821688493254273</v>
-      </c>
-      <c r="E49" s="2">
+      <c r="C49" s="1">
+        <f t="shared" si="0"/>
+        <v>5.3303892272536331</v>
+      </c>
+      <c r="D49" s="1">
+        <f t="shared" si="1"/>
+        <v>9.821688493254273</v>
+      </c>
+      <c r="E49" s="1">
         <f t="shared" si="2"/>
         <v>0.83908996125299318</v>
       </c>
@@ -4009,15 +4008,15 @@
       <c r="B50" s="1">
         <v>4.2577025708189895</v>
       </c>
-      <c r="C50">
-        <f t="shared" si="0"/>
-        <v>5.3303892272536331</v>
-      </c>
-      <c r="D50" s="2">
-        <f t="shared" si="1"/>
-        <v>9.821688493254273</v>
-      </c>
-      <c r="E50" s="2">
+      <c r="C50" s="1">
+        <f t="shared" si="0"/>
+        <v>5.3303892272536331</v>
+      </c>
+      <c r="D50" s="1">
+        <f t="shared" si="1"/>
+        <v>9.821688493254273</v>
+      </c>
+      <c r="E50" s="1">
         <f t="shared" si="2"/>
         <v>0.83908996125299318</v>
       </c>
@@ -4029,15 +4028,15 @@
       <c r="B51" s="1">
         <v>5.3110796807448581</v>
       </c>
-      <c r="C51">
-        <f t="shared" si="0"/>
-        <v>5.3303892272536331</v>
-      </c>
-      <c r="D51" s="2">
-        <f t="shared" si="1"/>
-        <v>9.821688493254273</v>
-      </c>
-      <c r="E51" s="2">
+      <c r="C51" s="1">
+        <f t="shared" si="0"/>
+        <v>5.3303892272536331</v>
+      </c>
+      <c r="D51" s="1">
+        <f t="shared" si="1"/>
+        <v>9.821688493254273</v>
+      </c>
+      <c r="E51" s="1">
         <f t="shared" si="2"/>
         <v>0.83908996125299318</v>
       </c>
@@ -4049,15 +4048,15 @@
       <c r="B52" s="1">
         <v>4.8742560969071134</v>
       </c>
-      <c r="C52">
-        <f t="shared" si="0"/>
-        <v>5.3303892272536331</v>
-      </c>
-      <c r="D52" s="2">
-        <f t="shared" si="1"/>
-        <v>9.821688493254273</v>
-      </c>
-      <c r="E52" s="2">
+      <c r="C52" s="1">
+        <f t="shared" si="0"/>
+        <v>5.3303892272536331</v>
+      </c>
+      <c r="D52" s="1">
+        <f t="shared" si="1"/>
+        <v>9.821688493254273</v>
+      </c>
+      <c r="E52" s="1">
         <f t="shared" si="2"/>
         <v>0.83908996125299318</v>
       </c>
@@ -4069,15 +4068,15 @@
       <c r="B53" s="1">
         <v>7.1094277399152759</v>
       </c>
-      <c r="C53">
-        <f t="shared" si="0"/>
-        <v>5.3303892272536331</v>
-      </c>
-      <c r="D53" s="2">
-        <f t="shared" si="1"/>
-        <v>9.821688493254273</v>
-      </c>
-      <c r="E53" s="2">
+      <c r="C53" s="1">
+        <f t="shared" si="0"/>
+        <v>5.3303892272536331</v>
+      </c>
+      <c r="D53" s="1">
+        <f t="shared" si="1"/>
+        <v>9.821688493254273</v>
+      </c>
+      <c r="E53" s="1">
         <f t="shared" si="2"/>
         <v>0.83908996125299318</v>
       </c>

</xml_diff>

<commit_message>
edit xlsx files added L3
</commit_message>
<xml_diff>
--- a/xlsx/L1-1.xlsx
+++ b/xlsx/L1-1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\QI-104\IHI-QI104\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F47CAC60-EFC2-428D-931B-802E46805E51}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6164F265-0904-4955-A34D-4FF1D411BB26}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,9 +38,6 @@
     <t>Week</t>
   </si>
   <si>
-    <t>perc</t>
-  </si>
-  <si>
     <t>UCL</t>
   </si>
   <si>
@@ -51,6 +48,9 @@
   </si>
   <si>
     <t>median</t>
+  </si>
+  <si>
+    <t>%</t>
   </si>
 </sst>
 </file>
@@ -86,9 +86,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -205,7 +210,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>perc</c:v>
+                  <c:v>%</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3002,52 +3007,54 @@
   <dimension ref="A1:H53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V5" sqref="V5"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2">
+        <v>5.1530413089687421</v>
+      </c>
+      <c r="C2" s="2">
+        <f>MEDIAN(B:B)</f>
+        <v>5.3303892272536331</v>
+      </c>
+      <c r="D2" s="2">
+        <f>H$3+(H$2* 3 )</f>
+        <v>9.821688493254273</v>
+      </c>
+      <c r="E2" s="2">
+        <f>H$3-(H$2* 3 )</f>
+        <v>0.83908996125299318</v>
+      </c>
+      <c r="G2" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1">
-        <v>5.1530413089687421</v>
-      </c>
-      <c r="C2" s="1">
-        <f>MEDIAN(B:B)</f>
-        <v>5.3303892272536331</v>
-      </c>
-      <c r="D2" s="1">
-        <f>H$3+(H$2* 3 )</f>
-        <v>9.821688493254273</v>
-      </c>
-      <c r="E2" s="1">
-        <f>H$3-(H$2* 3 )</f>
-        <v>0.83908996125299318</v>
-      </c>
-      <c r="G2" t="s">
-        <v>4</v>
       </c>
       <c r="H2">
         <f>STDEV(B2:B53)</f>
@@ -3055,26 +3062,26 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="2">
         <v>4.0954059070930224</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="2">
         <f t="shared" ref="C3:C53" si="0">MEDIAN(B:B)</f>
         <v>5.3303892272536331</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="2">
         <f t="shared" ref="D3:D53" si="1">H$3+(H$2* 3 )</f>
         <v>9.821688493254273</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3" s="2">
         <f t="shared" ref="E3:E53" si="2">H$3-(H$2* 3 )</f>
         <v>0.83908996125299318</v>
       </c>
       <c r="G3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H3">
         <f>MEDIAN(B:B)</f>
@@ -3082,1001 +3089,1001 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="2">
         <v>4.5943494198374673</v>
       </c>
-      <c r="C4" s="1">
-        <f t="shared" si="0"/>
-        <v>5.3303892272536331</v>
-      </c>
-      <c r="D4" s="1">
-        <f t="shared" si="1"/>
-        <v>9.821688493254273</v>
-      </c>
-      <c r="E4" s="1">
+      <c r="C4" s="2">
+        <f t="shared" si="0"/>
+        <v>5.3303892272536331</v>
+      </c>
+      <c r="D4" s="2">
+        <f t="shared" si="1"/>
+        <v>9.821688493254273</v>
+      </c>
+      <c r="E4" s="2">
         <f t="shared" si="2"/>
         <v>0.83908996125299318</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="2">
         <v>7.6393267019633271</v>
       </c>
-      <c r="C5" s="1">
-        <f t="shared" si="0"/>
-        <v>5.3303892272536331</v>
-      </c>
-      <c r="D5" s="1">
-        <f t="shared" si="1"/>
-        <v>9.821688493254273</v>
-      </c>
-      <c r="E5" s="1">
+      <c r="C5" s="2">
+        <f t="shared" si="0"/>
+        <v>5.3303892272536331</v>
+      </c>
+      <c r="D5" s="2">
+        <f t="shared" si="1"/>
+        <v>9.821688493254273</v>
+      </c>
+      <c r="E5" s="2">
         <f t="shared" si="2"/>
         <v>0.83908996125299318</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="2">
         <v>3.1005619085876628</v>
       </c>
-      <c r="C6" s="1">
-        <f t="shared" si="0"/>
-        <v>5.3303892272536331</v>
-      </c>
-      <c r="D6" s="1">
-        <f t="shared" si="1"/>
-        <v>9.821688493254273</v>
-      </c>
-      <c r="E6" s="1">
+      <c r="C6" s="2">
+        <f t="shared" si="0"/>
+        <v>5.3303892272536331</v>
+      </c>
+      <c r="D6" s="2">
+        <f t="shared" si="1"/>
+        <v>9.821688493254273</v>
+      </c>
+      <c r="E6" s="2">
         <f t="shared" si="2"/>
         <v>0.83908996125299318</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7">
+      <c r="A7" s="1">
         <v>6</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7" s="2">
         <v>5.3197840698422949</v>
       </c>
-      <c r="C7" s="1">
-        <f t="shared" si="0"/>
-        <v>5.3303892272536331</v>
-      </c>
-      <c r="D7" s="1">
-        <f t="shared" si="1"/>
-        <v>9.821688493254273</v>
-      </c>
-      <c r="E7" s="1">
+      <c r="C7" s="2">
+        <f t="shared" si="0"/>
+        <v>5.3303892272536331</v>
+      </c>
+      <c r="D7" s="2">
+        <f t="shared" si="1"/>
+        <v>9.821688493254273</v>
+      </c>
+      <c r="E7" s="2">
         <f t="shared" si="2"/>
         <v>0.83908996125299318</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="A8" s="1">
         <v>7</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8" s="2">
         <v>4.0665241452581107</v>
       </c>
-      <c r="C8" s="1">
-        <f t="shared" si="0"/>
-        <v>5.3303892272536331</v>
-      </c>
-      <c r="D8" s="1">
-        <f t="shared" si="1"/>
-        <v>9.821688493254273</v>
-      </c>
-      <c r="E8" s="1">
+      <c r="C8" s="2">
+        <f t="shared" si="0"/>
+        <v>5.3303892272536331</v>
+      </c>
+      <c r="D8" s="2">
+        <f t="shared" si="1"/>
+        <v>9.821688493254273</v>
+      </c>
+      <c r="E8" s="2">
         <f t="shared" si="2"/>
         <v>0.83908996125299318</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9">
+      <c r="A9" s="1">
         <v>8</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9" s="2">
         <v>7.2050144137075227</v>
       </c>
-      <c r="C9" s="1">
-        <f t="shared" si="0"/>
-        <v>5.3303892272536331</v>
-      </c>
-      <c r="D9" s="1">
-        <f t="shared" si="1"/>
-        <v>9.821688493254273</v>
-      </c>
-      <c r="E9" s="1">
+      <c r="C9" s="2">
+        <f t="shared" si="0"/>
+        <v>5.3303892272536331</v>
+      </c>
+      <c r="D9" s="2">
+        <f t="shared" si="1"/>
+        <v>9.821688493254273</v>
+      </c>
+      <c r="E9" s="2">
         <f t="shared" si="2"/>
         <v>0.83908996125299318</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10">
+      <c r="A10" s="1">
         <v>9</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10" s="2">
         <v>5.3409943846649703</v>
       </c>
-      <c r="C10" s="1">
-        <f t="shared" si="0"/>
-        <v>5.3303892272536331</v>
-      </c>
-      <c r="D10" s="1">
-        <f t="shared" si="1"/>
-        <v>9.821688493254273</v>
-      </c>
-      <c r="E10" s="1">
+      <c r="C10" s="2">
+        <f t="shared" si="0"/>
+        <v>5.3303892272536331</v>
+      </c>
+      <c r="D10" s="2">
+        <f t="shared" si="1"/>
+        <v>9.821688493254273</v>
+      </c>
+      <c r="E10" s="2">
         <f t="shared" si="2"/>
         <v>0.83908996125299318</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11">
+      <c r="A11" s="1">
         <v>10</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B11" s="2">
         <v>7.1482092027772826</v>
       </c>
-      <c r="C11" s="1">
-        <f t="shared" si="0"/>
-        <v>5.3303892272536331</v>
-      </c>
-      <c r="D11" s="1">
-        <f t="shared" si="1"/>
-        <v>9.821688493254273</v>
-      </c>
-      <c r="E11" s="1">
+      <c r="C11" s="2">
+        <f t="shared" si="0"/>
+        <v>5.3303892272536331</v>
+      </c>
+      <c r="D11" s="2">
+        <f t="shared" si="1"/>
+        <v>9.821688493254273</v>
+      </c>
+      <c r="E11" s="2">
         <f t="shared" si="2"/>
         <v>0.83908996125299318</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12">
+      <c r="A12" s="1">
         <v>11</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12" s="2">
         <v>3.8779734357075952</v>
       </c>
-      <c r="C12" s="1">
-        <f t="shared" si="0"/>
-        <v>5.3303892272536331</v>
-      </c>
-      <c r="D12" s="1">
-        <f t="shared" si="1"/>
-        <v>9.821688493254273</v>
-      </c>
-      <c r="E12" s="1">
+      <c r="C12" s="2">
+        <f t="shared" si="0"/>
+        <v>5.3303892272536331</v>
+      </c>
+      <c r="D12" s="2">
+        <f t="shared" si="1"/>
+        <v>9.821688493254273</v>
+      </c>
+      <c r="E12" s="2">
         <f t="shared" si="2"/>
         <v>0.83908996125299318</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13">
+      <c r="A13" s="1">
         <v>12</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B13" s="2">
         <v>3.3150046848766981</v>
       </c>
-      <c r="C13" s="1">
-        <f t="shared" si="0"/>
-        <v>5.3303892272536331</v>
-      </c>
-      <c r="D13" s="1">
-        <f t="shared" si="1"/>
-        <v>9.821688493254273</v>
-      </c>
-      <c r="E13" s="1">
+      <c r="C13" s="2">
+        <f t="shared" si="0"/>
+        <v>5.3303892272536331</v>
+      </c>
+      <c r="D13" s="2">
+        <f t="shared" si="1"/>
+        <v>9.821688493254273</v>
+      </c>
+      <c r="E13" s="2">
         <f t="shared" si="2"/>
         <v>0.83908996125299318</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14">
+      <c r="A14" s="1">
         <v>13</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B14" s="2">
         <v>7.555710089756869</v>
       </c>
-      <c r="C14" s="1">
-        <f t="shared" si="0"/>
-        <v>5.3303892272536331</v>
-      </c>
-      <c r="D14" s="1">
-        <f t="shared" si="1"/>
-        <v>9.821688493254273</v>
-      </c>
-      <c r="E14" s="1">
+      <c r="C14" s="2">
+        <f t="shared" si="0"/>
+        <v>5.3303892272536331</v>
+      </c>
+      <c r="D14" s="2">
+        <f t="shared" si="1"/>
+        <v>9.821688493254273</v>
+      </c>
+      <c r="E14" s="2">
         <f t="shared" si="2"/>
         <v>0.83908996125299318</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15">
+      <c r="A15" s="1">
         <v>14</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B15" s="2">
         <v>5.6396165788025368</v>
       </c>
-      <c r="C15" s="1">
-        <f t="shared" si="0"/>
-        <v>5.3303892272536331</v>
-      </c>
-      <c r="D15" s="1">
-        <f t="shared" si="1"/>
-        <v>9.821688493254273</v>
-      </c>
-      <c r="E15" s="1">
+      <c r="C15" s="2">
+        <f t="shared" si="0"/>
+        <v>5.3303892272536331</v>
+      </c>
+      <c r="D15" s="2">
+        <f t="shared" si="1"/>
+        <v>9.821688493254273</v>
+      </c>
+      <c r="E15" s="2">
         <f t="shared" si="2"/>
         <v>0.83908996125299318</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16">
+      <c r="A16" s="1">
         <v>15</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B16" s="2">
         <v>7.763306022315497</v>
       </c>
-      <c r="C16" s="1">
-        <f t="shared" si="0"/>
-        <v>5.3303892272536331</v>
-      </c>
-      <c r="D16" s="1">
-        <f t="shared" si="1"/>
-        <v>9.821688493254273</v>
-      </c>
-      <c r="E16" s="1">
+      <c r="C16" s="2">
+        <f t="shared" si="0"/>
+        <v>5.3303892272536331</v>
+      </c>
+      <c r="D16" s="2">
+        <f t="shared" si="1"/>
+        <v>9.821688493254273</v>
+      </c>
+      <c r="E16" s="2">
         <f t="shared" si="2"/>
         <v>0.83908996125299318</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17">
+      <c r="A17" s="1">
         <v>16</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B17" s="2">
         <v>5.4221224313444747</v>
       </c>
-      <c r="C17" s="1">
-        <f t="shared" si="0"/>
-        <v>5.3303892272536331</v>
-      </c>
-      <c r="D17" s="1">
-        <f t="shared" si="1"/>
-        <v>9.821688493254273</v>
-      </c>
-      <c r="E17" s="1">
+      <c r="C17" s="2">
+        <f t="shared" si="0"/>
+        <v>5.3303892272536331</v>
+      </c>
+      <c r="D17" s="2">
+        <f t="shared" si="1"/>
+        <v>9.821688493254273</v>
+      </c>
+      <c r="E17" s="2">
         <f t="shared" si="2"/>
         <v>0.83908996125299318</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18">
+      <c r="A18" s="1">
         <v>17</v>
       </c>
-      <c r="B18" s="1">
+      <c r="B18" s="2">
         <v>5.7552291383214058</v>
       </c>
-      <c r="C18" s="1">
-        <f t="shared" si="0"/>
-        <v>5.3303892272536331</v>
-      </c>
-      <c r="D18" s="1">
-        <f t="shared" si="1"/>
-        <v>9.821688493254273</v>
-      </c>
-      <c r="E18" s="1">
+      <c r="C18" s="2">
+        <f t="shared" si="0"/>
+        <v>5.3303892272536331</v>
+      </c>
+      <c r="D18" s="2">
+        <f t="shared" si="1"/>
+        <v>9.821688493254273</v>
+      </c>
+      <c r="E18" s="2">
         <f t="shared" si="2"/>
         <v>0.83908996125299318</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19">
+      <c r="A19" s="1">
         <v>18</v>
       </c>
-      <c r="B19" s="1">
+      <c r="B19" s="2">
         <v>6.8204787267303102</v>
       </c>
-      <c r="C19" s="1">
-        <f t="shared" si="0"/>
-        <v>5.3303892272536331</v>
-      </c>
-      <c r="D19" s="1">
-        <f t="shared" si="1"/>
-        <v>9.821688493254273</v>
-      </c>
-      <c r="E19" s="1">
+      <c r="C19" s="2">
+        <f t="shared" si="0"/>
+        <v>5.3303892272536331</v>
+      </c>
+      <c r="D19" s="2">
+        <f t="shared" si="1"/>
+        <v>9.821688493254273</v>
+      </c>
+      <c r="E19" s="2">
         <f t="shared" si="2"/>
         <v>0.83908996125299318</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20">
+      <c r="A20" s="1">
         <v>19</v>
       </c>
-      <c r="B20" s="1">
+      <c r="B20" s="2">
         <v>4.0759926522959651</v>
       </c>
-      <c r="C20" s="1">
-        <f t="shared" si="0"/>
-        <v>5.3303892272536331</v>
-      </c>
-      <c r="D20" s="1">
-        <f t="shared" si="1"/>
-        <v>9.821688493254273</v>
-      </c>
-      <c r="E20" s="1">
+      <c r="C20" s="2">
+        <f t="shared" si="0"/>
+        <v>5.3303892272536331</v>
+      </c>
+      <c r="D20" s="2">
+        <f t="shared" si="1"/>
+        <v>9.821688493254273</v>
+      </c>
+      <c r="E20" s="2">
         <f t="shared" si="2"/>
         <v>0.83908996125299318</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21">
+      <c r="A21" s="1">
         <v>20</v>
       </c>
-      <c r="B21" s="1">
+      <c r="B21" s="2">
         <v>3.2559808611488119</v>
       </c>
-      <c r="C21" s="1">
-        <f t="shared" si="0"/>
-        <v>5.3303892272536331</v>
-      </c>
-      <c r="D21" s="1">
-        <f t="shared" si="1"/>
-        <v>9.821688493254273</v>
-      </c>
-      <c r="E21" s="1">
+      <c r="C21" s="2">
+        <f t="shared" si="0"/>
+        <v>5.3303892272536331</v>
+      </c>
+      <c r="D21" s="2">
+        <f t="shared" si="1"/>
+        <v>9.821688493254273</v>
+      </c>
+      <c r="E21" s="2">
         <f t="shared" si="2"/>
         <v>0.83908996125299318</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22">
+      <c r="A22" s="1">
         <v>21</v>
       </c>
-      <c r="B22" s="1">
+      <c r="B22" s="2">
         <v>3.6746491065817146</v>
       </c>
-      <c r="C22" s="1">
-        <f t="shared" si="0"/>
-        <v>5.3303892272536331</v>
-      </c>
-      <c r="D22" s="1">
-        <f t="shared" si="1"/>
-        <v>9.821688493254273</v>
-      </c>
-      <c r="E22" s="1">
+      <c r="C22" s="2">
+        <f t="shared" si="0"/>
+        <v>5.3303892272536331</v>
+      </c>
+      <c r="D22" s="2">
+        <f t="shared" si="1"/>
+        <v>9.821688493254273</v>
+      </c>
+      <c r="E22" s="2">
         <f t="shared" si="2"/>
         <v>0.83908996125299318</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23">
+      <c r="A23" s="1">
         <v>22</v>
       </c>
-      <c r="B23" s="1">
+      <c r="B23" s="2">
         <v>6.8390627504248052</v>
       </c>
-      <c r="C23" s="1">
-        <f t="shared" si="0"/>
-        <v>5.3303892272536331</v>
-      </c>
-      <c r="D23" s="1">
-        <f t="shared" si="1"/>
-        <v>9.821688493254273</v>
-      </c>
-      <c r="E23" s="1">
+      <c r="C23" s="2">
+        <f t="shared" si="0"/>
+        <v>5.3303892272536331</v>
+      </c>
+      <c r="D23" s="2">
+        <f t="shared" si="1"/>
+        <v>9.821688493254273</v>
+      </c>
+      <c r="E23" s="2">
         <f t="shared" si="2"/>
         <v>0.83908996125299318</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24">
+      <c r="A24" s="1">
         <v>23</v>
       </c>
-      <c r="B24" s="1">
+      <c r="B24" s="2">
         <v>6.4681828082838617</v>
       </c>
-      <c r="C24" s="1">
-        <f t="shared" si="0"/>
-        <v>5.3303892272536331</v>
-      </c>
-      <c r="D24" s="1">
-        <f t="shared" si="1"/>
-        <v>9.821688493254273</v>
-      </c>
-      <c r="E24" s="1">
+      <c r="C24" s="2">
+        <f t="shared" si="0"/>
+        <v>5.3303892272536331</v>
+      </c>
+      <c r="D24" s="2">
+        <f t="shared" si="1"/>
+        <v>9.821688493254273</v>
+      </c>
+      <c r="E24" s="2">
         <f t="shared" si="2"/>
         <v>0.83908996125299318</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25">
+      <c r="A25" s="1">
         <v>24</v>
       </c>
-      <c r="B25" s="1">
+      <c r="B25" s="2">
         <v>7.8624827158895698</v>
       </c>
-      <c r="C25" s="1">
-        <f t="shared" si="0"/>
-        <v>5.3303892272536331</v>
-      </c>
-      <c r="D25" s="1">
-        <f t="shared" si="1"/>
-        <v>9.821688493254273</v>
-      </c>
-      <c r="E25" s="1">
+      <c r="C25" s="2">
+        <f t="shared" si="0"/>
+        <v>5.3303892272536331</v>
+      </c>
+      <c r="D25" s="2">
+        <f t="shared" si="1"/>
+        <v>9.821688493254273</v>
+      </c>
+      <c r="E25" s="2">
         <f t="shared" si="2"/>
         <v>0.83908996125299318</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26">
+      <c r="A26" s="1">
         <v>25</v>
       </c>
-      <c r="B26" s="1">
+      <c r="B26" s="2">
         <v>7.0583269308621883</v>
       </c>
-      <c r="C26" s="1">
-        <f t="shared" si="0"/>
-        <v>5.3303892272536331</v>
-      </c>
-      <c r="D26" s="1">
-        <f t="shared" si="1"/>
-        <v>9.821688493254273</v>
-      </c>
-      <c r="E26" s="1">
+      <c r="C26" s="2">
+        <f t="shared" si="0"/>
+        <v>5.3303892272536331</v>
+      </c>
+      <c r="D26" s="2">
+        <f t="shared" si="1"/>
+        <v>9.821688493254273</v>
+      </c>
+      <c r="E26" s="2">
         <f t="shared" si="2"/>
         <v>0.83908996125299318</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27">
+      <c r="A27" s="1">
         <v>26</v>
       </c>
-      <c r="B27" s="1">
+      <c r="B27" s="2">
         <v>3.5430589252308038</v>
       </c>
-      <c r="C27" s="1">
-        <f t="shared" si="0"/>
-        <v>5.3303892272536331</v>
-      </c>
-      <c r="D27" s="1">
-        <f t="shared" si="1"/>
-        <v>9.821688493254273</v>
-      </c>
-      <c r="E27" s="1">
+      <c r="C27" s="2">
+        <f t="shared" si="0"/>
+        <v>5.3303892272536331</v>
+      </c>
+      <c r="D27" s="2">
+        <f t="shared" si="1"/>
+        <v>9.821688493254273</v>
+      </c>
+      <c r="E27" s="2">
         <f t="shared" si="2"/>
         <v>0.83908996125299318</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28">
+      <c r="A28" s="1">
         <v>27</v>
       </c>
-      <c r="B28" s="1">
+      <c r="B28" s="2">
         <v>3.9447878457229946</v>
       </c>
-      <c r="C28" s="1">
-        <f t="shared" si="0"/>
-        <v>5.3303892272536331</v>
-      </c>
-      <c r="D28" s="1">
-        <f t="shared" si="1"/>
-        <v>9.821688493254273</v>
-      </c>
-      <c r="E28" s="1">
+      <c r="C28" s="2">
+        <f t="shared" si="0"/>
+        <v>5.3303892272536331</v>
+      </c>
+      <c r="D28" s="2">
+        <f t="shared" si="1"/>
+        <v>9.821688493254273</v>
+      </c>
+      <c r="E28" s="2">
         <f t="shared" si="2"/>
         <v>0.83908996125299318</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29">
+      <c r="A29" s="1">
         <v>28</v>
       </c>
-      <c r="B29" s="1">
+      <c r="B29" s="2">
         <v>6.3924618657014882</v>
       </c>
-      <c r="C29" s="1">
-        <f t="shared" si="0"/>
-        <v>5.3303892272536331</v>
-      </c>
-      <c r="D29" s="1">
-        <f t="shared" si="1"/>
-        <v>9.821688493254273</v>
-      </c>
-      <c r="E29" s="1">
+      <c r="C29" s="2">
+        <f t="shared" si="0"/>
+        <v>5.3303892272536331</v>
+      </c>
+      <c r="D29" s="2">
+        <f t="shared" si="1"/>
+        <v>9.821688493254273</v>
+      </c>
+      <c r="E29" s="2">
         <f t="shared" si="2"/>
         <v>0.83908996125299318</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30">
+      <c r="A30" s="1">
         <v>29</v>
       </c>
-      <c r="B30" s="1">
+      <c r="B30" s="2">
         <v>3.214380551268861</v>
       </c>
-      <c r="C30" s="1">
-        <f t="shared" si="0"/>
-        <v>5.3303892272536331</v>
-      </c>
-      <c r="D30" s="1">
-        <f t="shared" si="1"/>
-        <v>9.821688493254273</v>
-      </c>
-      <c r="E30" s="1">
+      <c r="C30" s="2">
+        <f t="shared" si="0"/>
+        <v>5.3303892272536331</v>
+      </c>
+      <c r="D30" s="2">
+        <f t="shared" si="1"/>
+        <v>9.821688493254273</v>
+      </c>
+      <c r="E30" s="2">
         <f t="shared" si="2"/>
         <v>0.83908996125299318</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31">
+      <c r="A31" s="1">
         <v>30</v>
       </c>
-      <c r="B31" s="1">
+      <c r="B31" s="2">
         <v>5.8113515624273209</v>
       </c>
-      <c r="C31" s="1">
-        <f t="shared" si="0"/>
-        <v>5.3303892272536331</v>
-      </c>
-      <c r="D31" s="1">
-        <f t="shared" si="1"/>
-        <v>9.821688493254273</v>
-      </c>
-      <c r="E31" s="1">
+      <c r="C31" s="2">
+        <f t="shared" si="0"/>
+        <v>5.3303892272536331</v>
+      </c>
+      <c r="D31" s="2">
+        <f t="shared" si="1"/>
+        <v>9.821688493254273</v>
+      </c>
+      <c r="E31" s="2">
         <f t="shared" si="2"/>
         <v>0.83908996125299318</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32">
+      <c r="A32" s="1">
         <v>31</v>
       </c>
-      <c r="B32" s="1">
+      <c r="B32" s="2">
         <v>6.6638751184812497</v>
       </c>
-      <c r="C32" s="1">
-        <f t="shared" si="0"/>
-        <v>5.3303892272536331</v>
-      </c>
-      <c r="D32" s="1">
-        <f t="shared" si="1"/>
-        <v>9.821688493254273</v>
-      </c>
-      <c r="E32" s="1">
+      <c r="C32" s="2">
+        <f t="shared" si="0"/>
+        <v>5.3303892272536331</v>
+      </c>
+      <c r="D32" s="2">
+        <f t="shared" si="1"/>
+        <v>9.821688493254273</v>
+      </c>
+      <c r="E32" s="2">
         <f t="shared" si="2"/>
         <v>0.83908996125299318</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33">
+      <c r="A33" s="1">
         <v>32</v>
       </c>
-      <c r="B33" s="1">
+      <c r="B33" s="2">
         <v>7.6934256538946606</v>
       </c>
-      <c r="C33" s="1">
-        <f t="shared" si="0"/>
-        <v>5.3303892272536331</v>
-      </c>
-      <c r="D33" s="1">
-        <f t="shared" si="1"/>
-        <v>9.821688493254273</v>
-      </c>
-      <c r="E33" s="1">
+      <c r="C33" s="2">
+        <f t="shared" si="0"/>
+        <v>5.3303892272536331</v>
+      </c>
+      <c r="D33" s="2">
+        <f t="shared" si="1"/>
+        <v>9.821688493254273</v>
+      </c>
+      <c r="E33" s="2">
         <f t="shared" si="2"/>
         <v>0.83908996125299318</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34">
+      <c r="A34" s="1">
         <v>33</v>
       </c>
-      <c r="B34" s="1">
+      <c r="B34" s="2">
         <v>3.916898026992877</v>
       </c>
-      <c r="C34" s="1">
-        <f t="shared" si="0"/>
-        <v>5.3303892272536331</v>
-      </c>
-      <c r="D34" s="1">
-        <f t="shared" si="1"/>
-        <v>9.821688493254273</v>
-      </c>
-      <c r="E34" s="1">
+      <c r="C34" s="2">
+        <f t="shared" si="0"/>
+        <v>5.3303892272536331</v>
+      </c>
+      <c r="D34" s="2">
+        <f t="shared" si="1"/>
+        <v>9.821688493254273</v>
+      </c>
+      <c r="E34" s="2">
         <f t="shared" si="2"/>
         <v>0.83908996125299318</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35">
+      <c r="A35" s="1">
         <v>34</v>
       </c>
-      <c r="B35" s="1">
+      <c r="B35" s="2">
         <v>5.9338158623080286</v>
       </c>
-      <c r="C35" s="1">
-        <f t="shared" si="0"/>
-        <v>5.3303892272536331</v>
-      </c>
-      <c r="D35" s="1">
-        <f t="shared" si="1"/>
-        <v>9.821688493254273</v>
-      </c>
-      <c r="E35" s="1">
+      <c r="C35" s="2">
+        <f t="shared" si="0"/>
+        <v>5.3303892272536331</v>
+      </c>
+      <c r="D35" s="2">
+        <f t="shared" si="1"/>
+        <v>9.821688493254273</v>
+      </c>
+      <c r="E35" s="2">
         <f t="shared" si="2"/>
         <v>0.83908996125299318</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36">
+      <c r="A36" s="1">
         <v>35</v>
       </c>
-      <c r="B36" s="1">
+      <c r="B36" s="2">
         <v>5.1056158240019922</v>
       </c>
-      <c r="C36" s="1">
-        <f t="shared" si="0"/>
-        <v>5.3303892272536331</v>
-      </c>
-      <c r="D36" s="1">
-        <f t="shared" si="1"/>
-        <v>9.821688493254273</v>
-      </c>
-      <c r="E36" s="1">
+      <c r="C36" s="2">
+        <f t="shared" si="0"/>
+        <v>5.3303892272536331</v>
+      </c>
+      <c r="D36" s="2">
+        <f t="shared" si="1"/>
+        <v>9.821688493254273</v>
+      </c>
+      <c r="E36" s="2">
         <f t="shared" si="2"/>
         <v>0.83908996125299318</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37">
+      <c r="A37" s="1">
         <v>36</v>
       </c>
-      <c r="B37" s="1">
+      <c r="B37" s="2">
         <v>4.0812833558478143</v>
       </c>
-      <c r="C37" s="1">
-        <f t="shared" si="0"/>
-        <v>5.3303892272536331</v>
-      </c>
-      <c r="D37" s="1">
-        <f t="shared" si="1"/>
-        <v>9.821688493254273</v>
-      </c>
-      <c r="E37" s="1">
+      <c r="C37" s="2">
+        <f t="shared" si="0"/>
+        <v>5.3303892272536331</v>
+      </c>
+      <c r="D37" s="2">
+        <f t="shared" si="1"/>
+        <v>9.821688493254273</v>
+      </c>
+      <c r="E37" s="2">
         <f t="shared" si="2"/>
         <v>0.83908996125299318</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38">
+      <c r="A38" s="1">
         <v>37</v>
       </c>
-      <c r="B38" s="1">
+      <c r="B38" s="2">
         <v>6.2744022206576773</v>
       </c>
-      <c r="C38" s="1">
-        <f t="shared" si="0"/>
-        <v>5.3303892272536331</v>
-      </c>
-      <c r="D38" s="1">
-        <f t="shared" si="1"/>
-        <v>9.821688493254273</v>
-      </c>
-      <c r="E38" s="1">
+      <c r="C38" s="2">
+        <f t="shared" si="0"/>
+        <v>5.3303892272536331</v>
+      </c>
+      <c r="D38" s="2">
+        <f t="shared" si="1"/>
+        <v>9.821688493254273</v>
+      </c>
+      <c r="E38" s="2">
         <f t="shared" si="2"/>
         <v>0.83908996125299318</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39">
+      <c r="A39" s="1">
         <v>38</v>
       </c>
-      <c r="B39" s="1">
+      <c r="B39" s="2">
         <v>3.8078765542056314</v>
       </c>
-      <c r="C39" s="1">
-        <f t="shared" si="0"/>
-        <v>5.3303892272536331</v>
-      </c>
-      <c r="D39" s="1">
-        <f t="shared" si="1"/>
-        <v>9.821688493254273</v>
-      </c>
-      <c r="E39" s="1">
+      <c r="C39" s="2">
+        <f t="shared" si="0"/>
+        <v>5.3303892272536331</v>
+      </c>
+      <c r="D39" s="2">
+        <f t="shared" si="1"/>
+        <v>9.821688493254273</v>
+      </c>
+      <c r="E39" s="2">
         <f t="shared" si="2"/>
         <v>0.83908996125299318</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40">
+      <c r="A40" s="1">
         <v>39</v>
       </c>
-      <c r="B40" s="1">
+      <c r="B40" s="2">
         <v>6.8501538724696456</v>
       </c>
-      <c r="C40" s="1">
-        <f t="shared" si="0"/>
-        <v>5.3303892272536331</v>
-      </c>
-      <c r="D40" s="1">
-        <f t="shared" si="1"/>
-        <v>9.821688493254273</v>
-      </c>
-      <c r="E40" s="1">
+      <c r="C40" s="2">
+        <f t="shared" si="0"/>
+        <v>5.3303892272536331</v>
+      </c>
+      <c r="D40" s="2">
+        <f t="shared" si="1"/>
+        <v>9.821688493254273</v>
+      </c>
+      <c r="E40" s="2">
         <f t="shared" si="2"/>
         <v>0.83908996125299318</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41">
+      <c r="A41" s="1">
         <v>40</v>
       </c>
-      <c r="B41" s="1">
+      <c r="B41" s="2">
         <v>4.828880642366161</v>
       </c>
-      <c r="C41" s="1">
-        <f t="shared" si="0"/>
-        <v>5.3303892272536331</v>
-      </c>
-      <c r="D41" s="1">
-        <f t="shared" si="1"/>
-        <v>9.821688493254273</v>
-      </c>
-      <c r="E41" s="1">
+      <c r="C41" s="2">
+        <f t="shared" si="0"/>
+        <v>5.3303892272536331</v>
+      </c>
+      <c r="D41" s="2">
+        <f t="shared" si="1"/>
+        <v>9.821688493254273</v>
+      </c>
+      <c r="E41" s="2">
         <f t="shared" si="2"/>
         <v>0.83908996125299318</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42">
+      <c r="A42" s="1">
         <v>41</v>
       </c>
-      <c r="B42" s="1">
+      <c r="B42" s="2">
         <v>6.9640933577555009</v>
       </c>
-      <c r="C42" s="1">
-        <f t="shared" si="0"/>
-        <v>5.3303892272536331</v>
-      </c>
-      <c r="D42" s="1">
-        <f t="shared" si="1"/>
-        <v>9.821688493254273</v>
-      </c>
-      <c r="E42" s="1">
+      <c r="C42" s="2">
+        <f t="shared" si="0"/>
+        <v>5.3303892272536331</v>
+      </c>
+      <c r="D42" s="2">
+        <f t="shared" si="1"/>
+        <v>9.821688493254273</v>
+      </c>
+      <c r="E42" s="2">
         <f t="shared" si="2"/>
         <v>0.83908996125299318</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43">
+      <c r="A43" s="1">
         <v>42</v>
       </c>
-      <c r="B43" s="1">
+      <c r="B43" s="2">
         <v>6.6508871810430383</v>
       </c>
-      <c r="C43" s="1">
-        <f t="shared" si="0"/>
-        <v>5.3303892272536331</v>
-      </c>
-      <c r="D43" s="1">
-        <f t="shared" si="1"/>
-        <v>9.821688493254273</v>
-      </c>
-      <c r="E43" s="1">
+      <c r="C43" s="2">
+        <f t="shared" si="0"/>
+        <v>5.3303892272536331</v>
+      </c>
+      <c r="D43" s="2">
+        <f t="shared" si="1"/>
+        <v>9.821688493254273</v>
+      </c>
+      <c r="E43" s="2">
         <f t="shared" si="2"/>
         <v>0.83908996125299318</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44">
+      <c r="A44" s="1">
         <v>43</v>
       </c>
-      <c r="B44" s="1">
+      <c r="B44" s="2">
         <v>4.2006919136498544</v>
       </c>
-      <c r="C44" s="1">
-        <f t="shared" si="0"/>
-        <v>5.3303892272536331</v>
-      </c>
-      <c r="D44" s="1">
-        <f t="shared" si="1"/>
-        <v>9.821688493254273</v>
-      </c>
-      <c r="E44" s="1">
+      <c r="C44" s="2">
+        <f t="shared" si="0"/>
+        <v>5.3303892272536331</v>
+      </c>
+      <c r="D44" s="2">
+        <f t="shared" si="1"/>
+        <v>9.821688493254273</v>
+      </c>
+      <c r="E44" s="2">
         <f t="shared" si="2"/>
         <v>0.83908996125299318</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45">
+      <c r="A45" s="1">
         <v>44</v>
       </c>
-      <c r="B45" s="1">
+      <c r="B45" s="2">
         <v>3.0337798814707018</v>
       </c>
-      <c r="C45" s="1">
-        <f t="shared" si="0"/>
-        <v>5.3303892272536331</v>
-      </c>
-      <c r="D45" s="1">
-        <f t="shared" si="1"/>
-        <v>9.821688493254273</v>
-      </c>
-      <c r="E45" s="1">
+      <c r="C45" s="2">
+        <f t="shared" si="0"/>
+        <v>5.3303892272536331</v>
+      </c>
+      <c r="D45" s="2">
+        <f t="shared" si="1"/>
+        <v>9.821688493254273</v>
+      </c>
+      <c r="E45" s="2">
         <f t="shared" si="2"/>
         <v>0.83908996125299318</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46">
+      <c r="A46" s="1">
         <v>45</v>
       </c>
-      <c r="B46" s="1">
+      <c r="B46" s="2">
         <v>6.9848003153180667</v>
       </c>
-      <c r="C46" s="1">
-        <f t="shared" si="0"/>
-        <v>5.3303892272536331</v>
-      </c>
-      <c r="D46" s="1">
-        <f t="shared" si="1"/>
-        <v>9.821688493254273</v>
-      </c>
-      <c r="E46" s="1">
+      <c r="C46" s="2">
+        <f t="shared" si="0"/>
+        <v>5.3303892272536331</v>
+      </c>
+      <c r="D46" s="2">
+        <f t="shared" si="1"/>
+        <v>9.821688493254273</v>
+      </c>
+      <c r="E46" s="2">
         <f t="shared" si="2"/>
         <v>0.83908996125299318</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47">
+      <c r="A47" s="1">
         <v>46</v>
       </c>
-      <c r="B47" s="1">
+      <c r="B47" s="2">
         <v>3.5676222447039212</v>
       </c>
-      <c r="C47" s="1">
-        <f t="shared" si="0"/>
-        <v>5.3303892272536331</v>
-      </c>
-      <c r="D47" s="1">
-        <f t="shared" si="1"/>
-        <v>9.821688493254273</v>
-      </c>
-      <c r="E47" s="1">
+      <c r="C47" s="2">
+        <f t="shared" si="0"/>
+        <v>5.3303892272536331</v>
+      </c>
+      <c r="D47" s="2">
+        <f t="shared" si="1"/>
+        <v>9.821688493254273</v>
+      </c>
+      <c r="E47" s="2">
         <f t="shared" si="2"/>
         <v>0.83908996125299318</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48">
+      <c r="A48" s="1">
         <v>47</v>
       </c>
-      <c r="B48" s="1">
+      <c r="B48" s="2">
         <v>5.2882081484461736</v>
       </c>
-      <c r="C48" s="1">
-        <f t="shared" si="0"/>
-        <v>5.3303892272536331</v>
-      </c>
-      <c r="D48" s="1">
-        <f t="shared" si="1"/>
-        <v>9.821688493254273</v>
-      </c>
-      <c r="E48" s="1">
+      <c r="C48" s="2">
+        <f t="shared" si="0"/>
+        <v>5.3303892272536331</v>
+      </c>
+      <c r="D48" s="2">
+        <f t="shared" si="1"/>
+        <v>9.821688493254273</v>
+      </c>
+      <c r="E48" s="2">
         <f t="shared" si="2"/>
         <v>0.83908996125299318</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49">
+      <c r="A49" s="1">
         <v>48</v>
       </c>
-      <c r="B49" s="1">
+      <c r="B49" s="2">
         <v>7.2069367492096408</v>
       </c>
-      <c r="C49" s="1">
-        <f t="shared" si="0"/>
-        <v>5.3303892272536331</v>
-      </c>
-      <c r="D49" s="1">
-        <f t="shared" si="1"/>
-        <v>9.821688493254273</v>
-      </c>
-      <c r="E49" s="1">
+      <c r="C49" s="2">
+        <f t="shared" si="0"/>
+        <v>5.3303892272536331</v>
+      </c>
+      <c r="D49" s="2">
+        <f t="shared" si="1"/>
+        <v>9.821688493254273</v>
+      </c>
+      <c r="E49" s="2">
         <f t="shared" si="2"/>
         <v>0.83908996125299318</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50">
+      <c r="A50" s="1">
         <v>49</v>
       </c>
-      <c r="B50" s="1">
+      <c r="B50" s="2">
         <v>4.2577025708189895</v>
       </c>
-      <c r="C50" s="1">
-        <f t="shared" si="0"/>
-        <v>5.3303892272536331</v>
-      </c>
-      <c r="D50" s="1">
-        <f t="shared" si="1"/>
-        <v>9.821688493254273</v>
-      </c>
-      <c r="E50" s="1">
+      <c r="C50" s="2">
+        <f t="shared" si="0"/>
+        <v>5.3303892272536331</v>
+      </c>
+      <c r="D50" s="2">
+        <f t="shared" si="1"/>
+        <v>9.821688493254273</v>
+      </c>
+      <c r="E50" s="2">
         <f t="shared" si="2"/>
         <v>0.83908996125299318</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51">
+      <c r="A51" s="1">
         <v>50</v>
       </c>
-      <c r="B51" s="1">
+      <c r="B51" s="2">
         <v>5.3110796807448581</v>
       </c>
-      <c r="C51" s="1">
-        <f t="shared" si="0"/>
-        <v>5.3303892272536331</v>
-      </c>
-      <c r="D51" s="1">
-        <f t="shared" si="1"/>
-        <v>9.821688493254273</v>
-      </c>
-      <c r="E51" s="1">
+      <c r="C51" s="2">
+        <f t="shared" si="0"/>
+        <v>5.3303892272536331</v>
+      </c>
+      <c r="D51" s="2">
+        <f t="shared" si="1"/>
+        <v>9.821688493254273</v>
+      </c>
+      <c r="E51" s="2">
         <f t="shared" si="2"/>
         <v>0.83908996125299318</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52">
+      <c r="A52" s="1">
         <v>51</v>
       </c>
-      <c r="B52" s="1">
+      <c r="B52" s="2">
         <v>4.8742560969071134</v>
       </c>
-      <c r="C52" s="1">
-        <f t="shared" si="0"/>
-        <v>5.3303892272536331</v>
-      </c>
-      <c r="D52" s="1">
-        <f t="shared" si="1"/>
-        <v>9.821688493254273</v>
-      </c>
-      <c r="E52" s="1">
+      <c r="C52" s="2">
+        <f t="shared" si="0"/>
+        <v>5.3303892272536331</v>
+      </c>
+      <c r="D52" s="2">
+        <f t="shared" si="1"/>
+        <v>9.821688493254273</v>
+      </c>
+      <c r="E52" s="2">
         <f t="shared" si="2"/>
         <v>0.83908996125299318</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53">
+      <c r="A53" s="1">
         <v>52</v>
       </c>
-      <c r="B53" s="1">
+      <c r="B53" s="2">
         <v>7.1094277399152759</v>
       </c>
-      <c r="C53" s="1">
-        <f t="shared" si="0"/>
-        <v>5.3303892272536331</v>
-      </c>
-      <c r="D53" s="1">
-        <f t="shared" si="1"/>
-        <v>9.821688493254273</v>
-      </c>
-      <c r="E53" s="1">
+      <c r="C53" s="2">
+        <f t="shared" si="0"/>
+        <v>5.3303892272536331</v>
+      </c>
+      <c r="D53" s="2">
+        <f t="shared" si="1"/>
+        <v>9.821688493254273</v>
+      </c>
+      <c r="E53" s="2">
         <f t="shared" si="2"/>
         <v>0.83908996125299318</v>
       </c>

</xml_diff>